<commit_message>
Linked lists: Remove nth node from the list - Done
</commit_message>
<xml_diff>
--- a/neetcode_150/neetcode150_fast_reviews.xlsx
+++ b/neetcode_150/neetcode150_fast_reviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mys1erious/Desktop/StudyProgramming/Git/algorithms/neetcode_150/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3F7E3D-7674-6443-9D14-6E84EB9C47A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1FEEB1-7FD6-B045-9010-2EEB6BA860CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="920" windowWidth="28040" windowHeight="17440" xr2:uid="{76CD3ECE-D592-4947-8368-191EE7B52C35}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>Arrays and Hashing</t>
   </si>
@@ -202,6 +202,33 @@
   </si>
   <si>
     <t>T: (2logn)</t>
+  </si>
+  <si>
+    <t>Merge 2 linked lists</t>
+  </si>
+  <si>
+    <t>T: O(n+m)</t>
+  </si>
+  <si>
+    <t>M: (n+m)</t>
+  </si>
+  <si>
+    <t>Add max(list1.val, list2.val) to result_list, change tail to tail.next, change listX to listX.next (X -&gt; list chosen from max func); when 1 of the lists ends, add the other to to tail.next; return result_list.next</t>
+  </si>
+  <si>
+    <t>Reorder linked list</t>
+  </si>
+  <si>
+    <t>Invery Binary Tree</t>
+  </si>
+  <si>
+    <t>Get middle of the list; reverse second half of the list; merge list1 with list2 by changing positions of lists on each iteration(list1.next = second, list2.next = tmp_first)</t>
+  </si>
+  <si>
+    <t>Remove nth from node</t>
+  </si>
+  <si>
+    <t>Add dummy node at the start of the list; init left to start of the list, init right to start+n); get to the end of the list shifting left and right by 1; make left.next = left.next.next</t>
   </si>
 </sst>
 </file>
@@ -425,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -437,12 +464,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -454,9 +475,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -506,35 +524,113 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,14 +638,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -560,64 +659,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -626,23 +680,26 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -958,84 +1015,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662B42D0-2FDD-8740-B5DE-63A10E0A48C3}">
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="8"/>
-    <col min="8" max="8" width="10.83203125" style="8"/>
-    <col min="17" max="17" width="10.83203125" style="8"/>
+    <col min="4" max="4" width="10.83203125" style="6"/>
+    <col min="8" max="8" width="10.83203125" style="6"/>
+    <col min="17" max="17" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43" t="s">
+      <c r="C1" s="65"/>
+      <c r="D1" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="42" t="s">
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="44" t="s">
+      <c r="C4" s="70"/>
+      <c r="D4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44" t="s">
+      <c r="E4" s="55"/>
+      <c r="F4" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="55"/>
+      <c r="H4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="4"/>
@@ -1047,402 +1104,453 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17">
+      <c r="A5" s="14">
         <v>2</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="50" t="s">
+      <c r="C5" s="70"/>
+      <c r="D5" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="44" t="s">
+      <c r="E5" s="54"/>
+      <c r="F5" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="52"/>
-      <c r="H5" s="45" t="s">
+      <c r="G5" s="56"/>
+      <c r="H5" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
     </row>
     <row r="6" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17">
+      <c r="A6" s="14">
         <v>3</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="50" t="s">
+      <c r="C6" s="70"/>
+      <c r="D6" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="44" t="s">
+      <c r="E6" s="54"/>
+      <c r="F6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="45" t="s">
+      <c r="G6" s="56"/>
+      <c r="H6" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="8" t="s">
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="9"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:17" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="69">
+      <c r="A13" s="29">
         <v>1</v>
       </c>
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="59" t="s">
+      <c r="C13" s="80"/>
+      <c r="D13" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="60"/>
-      <c r="F13" s="61" t="s">
+      <c r="E13" s="37"/>
+      <c r="F13" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="61"/>
-      <c r="H13" s="58" t="s">
+      <c r="G13" s="38"/>
+      <c r="H13" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="58"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
     </row>
     <row r="14" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
+      <c r="A14" s="14">
         <v>2</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="10"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="45" t="s">
+      <c r="H14" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="62"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="41"/>
     </row>
     <row r="15" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
     </row>
     <row r="16" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="17">
+      <c r="A16" s="14">
         <v>1</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="44" t="s">
+      <c r="C16" s="70"/>
+      <c r="D16" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44" t="s">
+      <c r="E16" s="55"/>
+      <c r="F16" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="8" t="s">
+      <c r="G16" s="55"/>
+      <c r="H16" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17">
+      <c r="A17" s="14">
         <v>2</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="9"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="H17" s="47" t="s">
+      <c r="H17" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
-      <c r="P17" s="49"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="72"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="72"/>
+      <c r="N17" s="72"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="73"/>
     </row>
     <row r="18" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="17">
+      <c r="A18" s="14">
         <v>3</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="76" t="s">
+      <c r="C18" s="70"/>
+      <c r="D18" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="67"/>
-      <c r="F18" s="66" t="s">
+      <c r="E18" s="46"/>
+      <c r="F18" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="77"/>
-      <c r="H18" s="45" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="62"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="41"/>
     </row>
     <row r="19" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="72">
+      <c r="A19" s="30">
         <v>4</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="73" t="s">
+      <c r="C19" s="70"/>
+      <c r="D19" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="74"/>
-      <c r="F19" s="68" t="s">
+      <c r="E19" s="48"/>
+      <c r="F19" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="75"/>
-      <c r="H19" s="45" t="s">
+      <c r="G19" s="50"/>
+      <c r="H19" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="62"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="41"/>
     </row>
     <row r="20" spans="1:16" ht="26" x14ac:dyDescent="0.2">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
+      <c r="A21" s="85">
         <v>1</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="65" t="s">
+      <c r="C21" s="87"/>
+      <c r="D21" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65" t="s">
+      <c r="E21" s="44"/>
+      <c r="F21" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="65"/>
-      <c r="H21" s="8" t="s">
+      <c r="G21" s="44"/>
+      <c r="H21" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="11"/>
+    <row r="22" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="32">
+        <v>2</v>
+      </c>
+      <c r="B22" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="80"/>
+      <c r="D22" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="63"/>
+      <c r="F22" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="64"/>
+      <c r="H22" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="41"/>
+    </row>
+    <row r="23" spans="1:16" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33">
+        <v>3</v>
+      </c>
+      <c r="B23" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="70"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:16" ht="26" x14ac:dyDescent="0.2">
-      <c r="A24" s="32" t="s">
+      <c r="H23" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="41"/>
+    </row>
+    <row r="24" spans="1:16" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="34">
+        <v>4</v>
+      </c>
+      <c r="B24" s="75" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="76"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="41"/>
+    </row>
+    <row r="25" spans="1:16" ht="26" x14ac:dyDescent="0.25">
+      <c r="A25" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="11"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="11"/>
+      <c r="A26" s="31">
+        <v>1</v>
+      </c>
+      <c r="B26" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="78"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:16" ht="26" x14ac:dyDescent="0.2">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:16" ht="26" x14ac:dyDescent="0.25">
+      <c r="A28" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-    </row>
-    <row r="28" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="11"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
@@ -1450,29 +1558,29 @@
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="11"/>
+      <c r="D29" s="9"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:16" ht="26" x14ac:dyDescent="0.2">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" spans="1:16" ht="26" x14ac:dyDescent="0.25">
+      <c r="A31" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-    </row>
-    <row r="31" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="11"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="9"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
@@ -1480,29 +1588,29 @@
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="11"/>
+      <c r="D32" s="9"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+    </row>
+    <row r="34" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A34" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-    </row>
-    <row r="34" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="11"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
@@ -1510,63 +1618,63 @@
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="11"/>
+      <c r="D35" s="9"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+    </row>
+    <row r="37" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A37" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-    </row>
-    <row r="37" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A37" s="22">
-        <v>1</v>
-      </c>
-      <c r="B37" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="11"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="9"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="11"/>
+      <c r="A38" s="19">
+        <v>1</v>
+      </c>
+      <c r="B38" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="82"/>
+      <c r="D38" s="9"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+    </row>
+    <row r="40" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A40" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-    </row>
-    <row r="40" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="11"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="9"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
@@ -1574,100 +1682,100 @@
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="11"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+    </row>
+    <row r="43" spans="1:17" s="23" customFormat="1" ht="26" x14ac:dyDescent="0.25">
+      <c r="A43" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="32"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-    </row>
-    <row r="43" spans="1:17" s="26" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A43" s="23">
+      <c r="B43" s="68"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="43"/>
+      <c r="F43" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="60"/>
+      <c r="H43" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q43" s="24"/>
+    </row>
+    <row r="44" spans="1:17" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="20">
         <v>1</v>
       </c>
-      <c r="B43" s="35" t="s">
+      <c r="B44" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="36"/>
-      <c r="D43" s="63" t="s">
+      <c r="C44" s="78"/>
+      <c r="D44" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="64"/>
-      <c r="F43" s="55" t="s">
+      <c r="E44" s="58"/>
+      <c r="F44" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="56"/>
-      <c r="H43" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q43" s="27"/>
-    </row>
-    <row r="44" spans="1:17" s="26" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A44" s="28">
+      <c r="G44" s="61"/>
+      <c r="H44" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q44" s="24"/>
+    </row>
+    <row r="45" spans="1:17" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A45" s="25">
         <v>2</v>
       </c>
-      <c r="B44" s="29" t="s">
+      <c r="B45" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="G44" s="57"/>
-      <c r="H44" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q44" s="27"/>
-    </row>
-    <row r="45" spans="1:17" s="26" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A45" s="25">
+      <c r="C45" s="26"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="24"/>
+      <c r="Q45" s="24"/>
+    </row>
+    <row r="46" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A46" s="22">
         <v>3</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B46" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="27"/>
-      <c r="Q45" s="27"/>
-    </row>
-    <row r="46" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A46" s="32" t="s">
+      <c r="C46" s="21"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+    </row>
+    <row r="47" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A47" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="32"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-    </row>
-    <row r="47" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="11"/>
+      <c r="B47" s="68"/>
+      <c r="C47" s="74"/>
+      <c r="D47" s="9"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
@@ -1675,122 +1783,139 @@
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="11"/>
+      <c r="D48" s="9"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:10" ht="26" x14ac:dyDescent="0.2">
-      <c r="A49" s="32" t="s">
+    <row r="49" spans="1:10" ht="26" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+    </row>
+    <row r="50" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+      <c r="A50" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="32"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-    </row>
-    <row r="50" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A50" s="24">
+      <c r="B50" s="68"/>
+      <c r="C50" s="74"/>
+    </row>
+    <row r="51" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A51" s="21">
         <v>1</v>
       </c>
-      <c r="B50" s="35" t="s">
+      <c r="B51" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="C50" s="36"/>
-    </row>
-    <row r="51" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="1:10" ht="26" x14ac:dyDescent="0.2">
-      <c r="A52" s="32" t="s">
+      <c r="C51" s="78"/>
+    </row>
+    <row r="52" spans="1:10" ht="26" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+    </row>
+    <row r="53" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+      <c r="A53" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="32"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-    </row>
-    <row r="53" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="B53" s="68"/>
+      <c r="C53" s="74"/>
     </row>
     <row r="54" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="1:10" ht="26" x14ac:dyDescent="0.2">
-      <c r="A55" s="32" t="s">
+    <row r="55" spans="1:10" ht="26" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+    </row>
+    <row r="56" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+      <c r="A56" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="32"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
+      <c r="B56" s="68"/>
+      <c r="C56" s="74"/>
     </row>
     <row r="58" spans="1:10" ht="26" x14ac:dyDescent="0.2">
-      <c r="A58" s="32" t="s">
+      <c r="D58" s="10"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+    </row>
+    <row r="59" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+      <c r="A59" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="B58" s="32"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-    </row>
-    <row r="59" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
+      <c r="B59" s="68"/>
+      <c r="C59" s="74"/>
     </row>
     <row r="60" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
+    <row r="61" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="H13:P13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H14:P14"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H18:P18"/>
-    <mergeCell ref="H19:P19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
+  <mergeCells count="71">
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="H1:J2"/>
     <mergeCell ref="D1:G2"/>
     <mergeCell ref="A3:C3"/>
@@ -1807,32 +1932,31 @@
     <mergeCell ref="H5:P5"/>
     <mergeCell ref="H17:P17"/>
     <mergeCell ref="H6:P6"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H13:P13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H14:P14"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H18:P18"/>
+    <mergeCell ref="H19:P19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H22:P22"/>
+    <mergeCell ref="H23:P23"/>
+    <mergeCell ref="H24:P24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
valid anagrams optimized and group_anagrams brute-force solutions
</commit_message>
<xml_diff>
--- a/neetcode_150/neetcode150_fast_reviews.xlsx
+++ b/neetcode_150/neetcode150_fast_reviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mys1erious/Desktop/StudyProgramming/Git/algorithms/neetcode_150/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF986F2-EFE1-7B4A-8DCD-D0BC6AB21EAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5045D42B-EE96-9B44-BF4D-38B72143174A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="920" windowWidth="28040" windowHeight="17440" xr2:uid="{76CD3ECE-D592-4947-8368-191EE7B52C35}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>Arrays and Hashing</t>
   </si>
@@ -72,9 +72,6 @@
     <t>M: O(n)</t>
   </si>
   <si>
-    <t>Make hashtable, add to it (value, 1) until u don’t get a duplicate, if u get a duplicate return True</t>
-  </si>
-  <si>
     <t>T: O(logn)</t>
   </si>
   <si>
@@ -160,12 +157,6 @@
   </si>
   <si>
     <t>Min cost climbing stairs</t>
-  </si>
-  <si>
-    <t>u check if str.len is the same in both words else return false; then u make 2 hashmaps for w1, w2 and make key=letter, val=num how many times its appeared in the word; then u compare those hashmaps</t>
-  </si>
-  <si>
-    <t>make a hashmap where key=arr.val, value=arr.ind; loop through the array and  check if target-arr[i] in hashmap, if its -&gt; return (arr[i], hashmap[arr[i]]), else add arr[i] to hashmap</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -312,6 +303,24 @@
   </si>
   <si>
     <t>Diameter of B.T</t>
+  </si>
+  <si>
+    <t>Make hashtable, add to it (value, index) until u don’t get a duplicate, if u get a duplicate return True</t>
+  </si>
+  <si>
+    <t>u check if str.len is the same in both words else return false; then u make 2 hashmaps for w1, w2 and make key=char, val=count; then u compare those hashmaps</t>
+  </si>
+  <si>
+    <t>make a hashmap where key=num, value=ind; loop through the array, if cur num not in hashmap - add it, check if target-num in hashmap, if its -&gt; return (ind, hashmap[target-num])</t>
+  </si>
+  <si>
+    <t>Group Anagrams</t>
+  </si>
+  <si>
+    <t>T: O(n*m)</t>
+  </si>
+  <si>
+    <t>M: O(n*m)</t>
   </si>
 </sst>
 </file>
@@ -541,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -675,6 +684,162 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -690,18 +855,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -711,154 +864,31 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1175,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662B42D0-2FDD-8740-B5DE-63A10E0A48C3}">
-  <dimension ref="A1:Q63"/>
+  <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:C29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1191,43 +1221,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="87" t="s">
+      <c r="C1" s="76"/>
+      <c r="D1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="86" t="s">
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="12"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -1240,20 +1270,20 @@
       <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="62" t="s">
+      <c r="C4" s="63"/>
+      <c r="D4" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62" t="s">
+      <c r="E4" s="78"/>
+      <c r="F4" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="62"/>
+      <c r="G4" s="78"/>
       <c r="H4" s="5" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -1267,87 +1297,91 @@
       <c r="A5" s="14">
         <v>2</v>
       </c>
-      <c r="B5" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="60" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="63"/>
-      <c r="H5" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
-      <c r="P5" s="68"/>
+      <c r="B5" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="63"/>
+      <c r="D5" s="84" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="85"/>
+      <c r="F5" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="86"/>
+      <c r="H5" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
     </row>
     <row r="6" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>3</v>
       </c>
-      <c r="B6" s="90" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="91"/>
-      <c r="D6" s="60" t="s">
+      <c r="B6" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="63"/>
+      <c r="D6" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62" t="s">
+      <c r="E6" s="85"/>
+      <c r="F6" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="63"/>
-      <c r="H6" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
       <c r="Q6" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
+      <c r="A7" s="121">
+        <v>4</v>
+      </c>
+      <c r="B7" s="122" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="123"/>
       <c r="D7" s="7"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="88" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="120"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
+      <c r="A9" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="64"/>
+      <c r="C9" s="119"/>
       <c r="D9" s="17"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
@@ -1357,11 +1391,9 @@
       <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="88" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="12"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -1371,9 +1403,11 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
+      <c r="A11" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="119"/>
       <c r="D11" s="17"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
@@ -1383,11 +1417,9 @@
       <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="89" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="89"/>
-      <c r="C12" s="95"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="10"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -1397,63 +1429,63 @@
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:17" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27">
+      <c r="A13" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="117"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="113" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="114"/>
+      <c r="F13" s="114" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="114"/>
+      <c r="H13" s="112" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="112"/>
+      <c r="N13" s="112"/>
+      <c r="O13" s="112"/>
+      <c r="P13" s="112"/>
+    </row>
+    <row r="14" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27">
         <v>1</v>
       </c>
-      <c r="B13" s="100" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="101"/>
-      <c r="D13" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="66"/>
-      <c r="H13" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="64"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="64"/>
-      <c r="P13" s="64"/>
-    </row>
-    <row r="14" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>2</v>
-      </c>
-      <c r="B14" s="90" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="91"/>
+      <c r="B14" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="61"/>
       <c r="D14" s="8"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="68"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="68"/>
-      <c r="O14" s="68"/>
-      <c r="P14" s="69"/>
+      <c r="H14" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="80"/>
+      <c r="P14" s="97"/>
     </row>
     <row r="15" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A15" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
+      <c r="A15" s="14">
+        <v>2</v>
+      </c>
+      <c r="B15" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="63"/>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -1463,115 +1495,115 @@
       <c r="J15" s="13"/>
     </row>
     <row r="16" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14">
-        <v>1</v>
-      </c>
-      <c r="B16" s="90" t="s">
+      <c r="A16" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="91"/>
-      <c r="D16" s="62" t="s">
+      <c r="B16" s="115"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="62"/>
+      <c r="G16" s="78"/>
       <c r="H16" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
-        <v>2</v>
-      </c>
-      <c r="B17" s="90" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="91"/>
-      <c r="D17" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="63"/>
+      <c r="D17" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="85"/>
+      <c r="F17" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="61"/>
-      <c r="F17" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="63"/>
-      <c r="H17" s="92" t="s">
-        <v>49</v>
-      </c>
-      <c r="I17" s="93"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="93"/>
-      <c r="L17" s="93"/>
-      <c r="M17" s="93"/>
-      <c r="N17" s="93"/>
-      <c r="O17" s="93"/>
-      <c r="P17" s="94"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="81" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="82"/>
+      <c r="P17" s="83"/>
     </row>
     <row r="18" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14">
+        <v>2</v>
+      </c>
+      <c r="B18" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="63"/>
+      <c r="D18" s="95" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="96"/>
+      <c r="F18" s="102" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="103"/>
+      <c r="H18" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="80"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="80"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="80"/>
+      <c r="N18" s="80"/>
+      <c r="O18" s="80"/>
+      <c r="P18" s="97"/>
+    </row>
+    <row r="19" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
         <v>3</v>
       </c>
-      <c r="B18" s="90" t="s">
+      <c r="B19" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="63"/>
+      <c r="D19" s="98" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="99"/>
+      <c r="F19" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="101"/>
+      <c r="H19" s="79" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="80"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="80"/>
+      <c r="O19" s="80"/>
+      <c r="P19" s="97"/>
+    </row>
+    <row r="20" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+      <c r="A20" s="28">
+        <v>4</v>
+      </c>
+      <c r="B20" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="91"/>
-      <c r="D18" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="74"/>
-      <c r="F18" s="79" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="80"/>
-      <c r="H18" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="68"/>
-      <c r="N18" s="68"/>
-      <c r="O18" s="68"/>
-      <c r="P18" s="69"/>
-    </row>
-    <row r="19" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28">
-        <v>4</v>
-      </c>
-      <c r="B19" s="90" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="91"/>
-      <c r="D19" s="75" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="76"/>
-      <c r="F19" s="77" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="78"/>
-      <c r="H19" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
-      <c r="M19" s="68"/>
-      <c r="N19" s="68"/>
-      <c r="O19" s="68"/>
-      <c r="P19" s="69"/>
-    </row>
-    <row r="20" spans="1:16" ht="26" x14ac:dyDescent="0.2">
-      <c r="A20" s="89" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="89"/>
-      <c r="C20" s="89"/>
+      <c r="C20" s="63"/>
       <c r="D20" s="10"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -1581,106 +1613,106 @@
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36">
+      <c r="A21" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="93"/>
+      <c r="F21" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="93"/>
+      <c r="H21" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="36">
         <v>1</v>
       </c>
-      <c r="B21" s="98" t="s">
+      <c r="B22" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="99"/>
-      <c r="D21" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="72"/>
-      <c r="H21" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29">
+      <c r="C22" s="71"/>
+      <c r="D22" s="91" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="92"/>
+      <c r="F22" s="93" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="94"/>
+      <c r="H22" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="80"/>
+      <c r="N22" s="80"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="97"/>
+    </row>
+    <row r="23" spans="1:16" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="29">
         <v>2</v>
       </c>
-      <c r="B22" s="100" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="83" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="84"/>
-      <c r="F22" s="72" t="s">
-        <v>58</v>
-      </c>
-      <c r="G22" s="85"/>
-      <c r="H22" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="68"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="68"/>
-      <c r="O22" s="68"/>
-      <c r="P22" s="69"/>
-    </row>
-    <row r="23" spans="1:16" ht="38" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30">
-        <v>3</v>
-      </c>
-      <c r="B23" s="90" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="91"/>
+      <c r="B23" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="61"/>
       <c r="D23" s="9"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="H23" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="68"/>
-      <c r="L23" s="68"/>
-      <c r="M23" s="68"/>
-      <c r="N23" s="68"/>
-      <c r="O23" s="68"/>
-      <c r="P23" s="69"/>
+      <c r="H23" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="80"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="97"/>
     </row>
     <row r="24" spans="1:16" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="31">
-        <v>4</v>
-      </c>
-      <c r="B24" s="102" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="102"/>
+      <c r="A24" s="30">
+        <v>3</v>
+      </c>
+      <c r="B24" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="63"/>
       <c r="D24" s="41"/>
       <c r="E24" s="42"/>
       <c r="F24" s="42"/>
       <c r="G24" s="44"/>
-      <c r="H24" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="68"/>
-      <c r="O24" s="68"/>
-      <c r="P24" s="69"/>
-    </row>
-    <row r="25" spans="1:16" ht="26" x14ac:dyDescent="0.25">
-      <c r="A25" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="96"/>
-      <c r="C25" s="97"/>
+      <c r="H24" s="80" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
+      <c r="K24" s="80"/>
+      <c r="L24" s="80"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="80"/>
+      <c r="P24" s="97"/>
+    </row>
+    <row r="25" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="31">
+        <v>4</v>
+      </c>
+      <c r="B25" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="72"/>
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
       <c r="F25" s="46"/>
@@ -1689,94 +1721,92 @@
       <c r="I25" s="49"/>
       <c r="J25" s="49"/>
     </row>
-    <row r="26" spans="1:16" ht="19" x14ac:dyDescent="0.2">
-      <c r="A26" s="35">
+    <row r="26" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+      <c r="A26" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="58"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="92"/>
+      <c r="F26" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="94"/>
+      <c r="H26" s="107" t="s">
+        <v>61</v>
+      </c>
+      <c r="I26" s="107"/>
+      <c r="J26" s="107"/>
+      <c r="K26" s="107"/>
+      <c r="L26" s="107"/>
+      <c r="M26" s="107"/>
+      <c r="N26" s="107"/>
+      <c r="O26" s="107"/>
+      <c r="P26" s="108"/>
+    </row>
+    <row r="27" spans="1:16" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="35">
         <v>1</v>
       </c>
-      <c r="B26" s="102" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="103"/>
-      <c r="D26" s="83" t="s">
+      <c r="B27" s="72" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="73"/>
+      <c r="D27" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="84"/>
-      <c r="F26" s="83" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="85"/>
-      <c r="H26" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="56"/>
-    </row>
-    <row r="27" spans="1:16" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="34">
+      <c r="E27" s="92"/>
+      <c r="F27" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="92"/>
+      <c r="H27" s="109" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" s="110"/>
+      <c r="J27" s="110"/>
+      <c r="K27" s="110"/>
+      <c r="L27" s="110"/>
+      <c r="M27" s="110"/>
+      <c r="N27" s="110"/>
+      <c r="O27" s="110"/>
+      <c r="P27" s="111"/>
+    </row>
+    <row r="28" spans="1:16" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="34">
         <v>2</v>
       </c>
-      <c r="B27" s="102" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="103"/>
-      <c r="D27" s="83" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="84"/>
-      <c r="F27" s="83" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="84"/>
-      <c r="H27" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="I27" s="58"/>
-      <c r="J27" s="58"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
-      <c r="O27" s="58"/>
-      <c r="P27" s="59"/>
-    </row>
-    <row r="28" spans="1:16" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="54">
-        <v>3</v>
-      </c>
-      <c r="B28" s="112" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="113"/>
+      <c r="B28" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="73"/>
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
       <c r="F28" s="33"/>
       <c r="G28" s="53"/>
-      <c r="H28" s="109" t="s">
-        <v>68</v>
-      </c>
-      <c r="I28" s="110"/>
-      <c r="J28" s="110"/>
-      <c r="K28" s="110"/>
-      <c r="L28" s="110"/>
-      <c r="M28" s="110"/>
-      <c r="N28" s="110"/>
-      <c r="O28" s="110"/>
-      <c r="P28" s="111"/>
+      <c r="H28" s="104" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" s="105"/>
+      <c r="J28" s="105"/>
+      <c r="K28" s="105"/>
+      <c r="L28" s="105"/>
+      <c r="M28" s="105"/>
+      <c r="N28" s="105"/>
+      <c r="O28" s="105"/>
+      <c r="P28" s="106"/>
     </row>
     <row r="29" spans="1:16" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37">
-        <v>4</v>
-      </c>
-      <c r="B29" s="115" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="116"/>
+      <c r="A29" s="54">
+        <v>3</v>
+      </c>
+      <c r="B29" s="74" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="75"/>
       <c r="D29" s="38"/>
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
@@ -1789,14 +1819,16 @@
       <c r="M29" s="52"/>
       <c r="N29" s="52"/>
       <c r="O29" s="52"/>
-      <c r="P29" s="114"/>
-    </row>
-    <row r="30" spans="1:16" ht="26" x14ac:dyDescent="0.25">
-      <c r="A30" s="89" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="89"/>
-      <c r="C30" s="95"/>
+      <c r="P29" s="55"/>
+    </row>
+    <row r="30" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="37">
+        <v>4</v>
+      </c>
+      <c r="B30" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="57"/>
       <c r="D30" s="46"/>
       <c r="E30" s="46"/>
       <c r="F30" s="46"/>
@@ -1811,10 +1843,12 @@
       <c r="O30" s="49"/>
       <c r="P30" s="47"/>
     </row>
-    <row r="31" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+    <row r="31" spans="1:16" ht="26" x14ac:dyDescent="0.25">
+      <c r="A31" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="58"/>
+      <c r="C31" s="59"/>
       <c r="D31" s="9"/>
       <c r="E31" s="43"/>
       <c r="F31" s="43"/>
@@ -1835,12 +1869,10 @@
       <c r="I32" s="42"/>
       <c r="J32" s="42"/>
     </row>
-    <row r="33" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A33" s="89" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="89"/>
-      <c r="C33" s="89"/>
+    <row r="33" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
       <c r="D33" s="43"/>
       <c r="E33" s="43"/>
       <c r="F33" s="43"/>
@@ -1849,10 +1881,12 @@
       <c r="I33" s="40"/>
       <c r="J33" s="40"/>
     </row>
-    <row r="34" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+    <row r="34" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A34" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="58"/>
+      <c r="C34" s="58"/>
       <c r="D34" s="43"/>
       <c r="E34" s="43"/>
       <c r="F34" s="43"/>
@@ -1873,12 +1907,10 @@
       <c r="I35" s="42"/>
       <c r="J35" s="42"/>
     </row>
-    <row r="36" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A36" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="89"/>
-      <c r="C36" s="89"/>
+    <row r="36" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
       <c r="D36" s="43"/>
       <c r="E36" s="43"/>
       <c r="F36" s="43"/>
@@ -1887,10 +1919,12 @@
       <c r="I36" s="40"/>
       <c r="J36" s="40"/>
     </row>
-    <row r="37" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+    <row r="37" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A37" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="58"/>
+      <c r="C37" s="58"/>
       <c r="D37" s="43"/>
       <c r="E37" s="43"/>
       <c r="F37" s="43"/>
@@ -1911,12 +1945,10 @@
       <c r="I38" s="42"/>
       <c r="J38" s="42"/>
     </row>
-    <row r="39" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A39" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="89"/>
-      <c r="C39" s="89"/>
+    <row r="39" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
       <c r="D39" s="43"/>
       <c r="E39" s="43"/>
       <c r="F39" s="43"/>
@@ -1925,14 +1957,12 @@
       <c r="I39" s="40"/>
       <c r="J39" s="40"/>
     </row>
-    <row r="40" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A40" s="19">
-        <v>1</v>
-      </c>
-      <c r="B40" s="107" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="108"/>
+    <row r="40" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A40" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="58"/>
+      <c r="C40" s="58"/>
       <c r="D40" s="43"/>
       <c r="E40" s="43"/>
       <c r="F40" s="43"/>
@@ -1942,9 +1972,13 @@
       <c r="J40" s="40"/>
     </row>
     <row r="41" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="A41" s="19">
+        <v>1</v>
+      </c>
+      <c r="B41" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="69"/>
       <c r="D41" s="42"/>
       <c r="E41" s="42"/>
       <c r="F41" s="42"/>
@@ -1953,12 +1987,10 @@
       <c r="I41" s="42"/>
       <c r="J41" s="42"/>
     </row>
-    <row r="42" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A42" s="89" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="89"/>
-      <c r="C42" s="89"/>
+    <row r="42" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
       <c r="D42" s="43"/>
       <c r="E42" s="43"/>
       <c r="F42" s="43"/>
@@ -1967,10 +1999,12 @@
       <c r="I42" s="40"/>
       <c r="J42" s="40"/>
     </row>
-    <row r="43" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+    <row r="43" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A43" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="58"/>
+      <c r="C43" s="58"/>
       <c r="D43" s="43"/>
       <c r="E43" s="43"/>
       <c r="F43" s="43"/>
@@ -1991,54 +2025,50 @@
       <c r="I44" s="42"/>
       <c r="J44" s="42"/>
     </row>
-    <row r="45" spans="1:17" s="23" customFormat="1" ht="26" x14ac:dyDescent="0.25">
-      <c r="A45" s="89" t="s">
-        <v>27</v>
-      </c>
-      <c r="B45" s="89"/>
-      <c r="C45" s="95"/>
-      <c r="D45" s="70" t="s">
+    <row r="45" spans="1:17" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="71"/>
-      <c r="F45" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="G45" s="82"/>
+      <c r="E45" s="88"/>
+      <c r="F45" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="90"/>
       <c r="H45" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q45" s="24"/>
+    </row>
+    <row r="46" spans="1:17" s="23" customFormat="1" ht="26" x14ac:dyDescent="0.25">
+      <c r="A46" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="58"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="88"/>
+      <c r="F46" s="88" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="90"/>
+      <c r="H46" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="Q45" s="24"/>
-    </row>
-    <row r="46" spans="1:17" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A46" s="20">
+      <c r="Q46" s="24"/>
+    </row>
+    <row r="47" spans="1:17" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A47" s="20">
         <v>1</v>
       </c>
-      <c r="B46" s="104" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="105"/>
-      <c r="D46" s="70" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="71"/>
-      <c r="F46" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="G46" s="82"/>
-      <c r="H46" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q46" s="24"/>
-    </row>
-    <row r="47" spans="1:17" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A47" s="25">
-        <v>2</v>
-      </c>
-      <c r="B47" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" s="26"/>
+      <c r="B47" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="66"/>
       <c r="D47" s="32"/>
       <c r="E47" s="32"/>
       <c r="F47" s="32"/>
@@ -2050,13 +2080,13 @@
       <c r="Q47" s="24"/>
     </row>
     <row r="48" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A48" s="22">
-        <v>3</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" s="21"/>
+      <c r="A48" s="25">
+        <v>2</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="26"/>
       <c r="D48" s="42"/>
       <c r="E48" s="42"/>
       <c r="F48" s="42"/>
@@ -2066,12 +2096,14 @@
       <c r="J48" s="42"/>
       <c r="K48" s="40"/>
     </row>
-    <row r="49" spans="1:11" ht="26" x14ac:dyDescent="0.25">
-      <c r="A49" s="89" t="s">
-        <v>28</v>
-      </c>
-      <c r="B49" s="89"/>
-      <c r="C49" s="89"/>
+    <row r="49" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A49" s="22">
+        <v>3</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="21"/>
       <c r="D49" s="43"/>
       <c r="E49" s="43"/>
       <c r="F49" s="43"/>
@@ -2081,10 +2113,12 @@
       <c r="J49" s="40"/>
       <c r="K49" s="40"/>
     </row>
-    <row r="50" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
+    <row r="50" spans="1:11" ht="26" x14ac:dyDescent="0.25">
+      <c r="A50" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" s="58"/>
+      <c r="C50" s="58"/>
       <c r="D50" s="43"/>
       <c r="E50" s="43"/>
       <c r="F50" s="43"/>
@@ -2107,12 +2141,10 @@
       <c r="J51" s="42"/>
       <c r="K51" s="40"/>
     </row>
-    <row r="52" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A52" s="89" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" s="89"/>
-      <c r="C52" s="89"/>
+    <row r="52" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
       <c r="D52" s="40"/>
       <c r="E52" s="40"/>
       <c r="F52" s="40"/>
@@ -2122,14 +2154,12 @@
       <c r="J52" s="40"/>
       <c r="K52" s="40"/>
     </row>
-    <row r="53" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A53" s="21">
-        <v>1</v>
-      </c>
-      <c r="B53" s="104" t="s">
-        <v>37</v>
-      </c>
-      <c r="C53" s="106"/>
+    <row r="53" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A53" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="58"/>
+      <c r="C53" s="58"/>
       <c r="D53" s="40"/>
       <c r="E53" s="40"/>
       <c r="F53" s="40"/>
@@ -2140,9 +2170,13 @@
       <c r="K53" s="40"/>
     </row>
     <row r="54" spans="1:11" ht="26" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="A54" s="21">
+        <v>1</v>
+      </c>
+      <c r="B54" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="67"/>
       <c r="D54" s="42"/>
       <c r="E54" s="42"/>
       <c r="F54" s="42"/>
@@ -2152,12 +2186,10 @@
       <c r="J54" s="42"/>
       <c r="K54" s="40"/>
     </row>
-    <row r="55" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A55" s="89" t="s">
-        <v>30</v>
-      </c>
-      <c r="B55" s="89"/>
-      <c r="C55" s="89"/>
+    <row r="55" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
       <c r="D55" s="40"/>
       <c r="E55" s="40"/>
       <c r="F55" s="40"/>
@@ -2167,10 +2199,12 @@
       <c r="J55" s="40"/>
       <c r="K55" s="40"/>
     </row>
-    <row r="56" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
+    <row r="56" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A56" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" s="58"/>
+      <c r="C56" s="58"/>
       <c r="D56" s="40"/>
       <c r="E56" s="40"/>
       <c r="F56" s="40"/>
@@ -2193,12 +2227,10 @@
       <c r="J57" s="42"/>
       <c r="K57" s="40"/>
     </row>
-    <row r="58" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A58" s="89" t="s">
-        <v>31</v>
-      </c>
-      <c r="B58" s="89"/>
-      <c r="C58" s="89"/>
+    <row r="58" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
       <c r="D58" s="40"/>
       <c r="E58" s="40"/>
       <c r="F58" s="40"/>
@@ -2208,7 +2240,12 @@
       <c r="J58" s="40"/>
       <c r="K58" s="40"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A59" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="58"/>
+      <c r="C59" s="58"/>
       <c r="D59" s="40"/>
       <c r="E59" s="40"/>
       <c r="F59" s="40"/>
@@ -2227,78 +2264,50 @@
       <c r="I60" s="42"/>
       <c r="J60" s="42"/>
     </row>
-    <row r="61" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A61" s="89" t="s">
-        <v>32</v>
-      </c>
-      <c r="B61" s="89"/>
-      <c r="C61" s="95"/>
-    </row>
-    <row r="62" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
+    <row r="62" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A62" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="58"/>
+      <c r="C62" s="59"/>
     </row>
     <row r="63" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
+    <row r="64" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="83">
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H1:J2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="H5:P5"/>
-    <mergeCell ref="H17:P17"/>
-    <mergeCell ref="H6:P6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
+  <mergeCells count="84">
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H13:P13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H14:P14"/>
+    <mergeCell ref="H22:P22"/>
+    <mergeCell ref="H23:P23"/>
+    <mergeCell ref="H24:P24"/>
+    <mergeCell ref="H28:P28"/>
+    <mergeCell ref="H26:P26"/>
+    <mergeCell ref="H27:P27"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H18:P18"/>
+    <mergeCell ref="H19:P19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="F46:G46"/>
@@ -2309,26 +2318,55 @@
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H18:P18"/>
-    <mergeCell ref="H19:P19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H22:P22"/>
-    <mergeCell ref="H23:P23"/>
-    <mergeCell ref="H24:P24"/>
-    <mergeCell ref="H28:P28"/>
-    <mergeCell ref="H26:P26"/>
-    <mergeCell ref="H27:P27"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H13:P13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H14:P14"/>
+    <mergeCell ref="H6:P6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="H1:J2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H5:P5"/>
+    <mergeCell ref="H17:P17"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
brute force solution for top k freq. elems
</commit_message>
<xml_diff>
--- a/neetcode_150/neetcode150_fast_reviews.xlsx
+++ b/neetcode_150/neetcode150_fast_reviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mys1erious/Desktop/StudyProgramming/Git/algorithms/neetcode_150/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5045D42B-EE96-9B44-BF4D-38B72143174A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3718A6DF-72EA-9748-BE70-C53ECD71DABA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="920" windowWidth="28040" windowHeight="17440" xr2:uid="{76CD3ECE-D592-4947-8368-191EE7B52C35}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
   <si>
     <t>Arrays and Hashing</t>
   </si>
@@ -321,6 +321,18 @@
   </si>
   <si>
     <t>M: O(n*m)</t>
+  </si>
+  <si>
+    <t>T: O(m*n*26)</t>
+  </si>
+  <si>
+    <t>M: O(m)</t>
+  </si>
+  <si>
+    <t>make an array of len 26 with 0s; count how many times each char appears in the str, add it to arr with ord(); make hm key:tuple(arr) val:arr(anagrams)</t>
+  </si>
+  <si>
+    <t>Top k Freq. Elements</t>
   </si>
 </sst>
 </file>
@@ -550,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -566,9 +578,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -687,11 +696,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -699,52 +720,43 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -753,7 +765,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -772,15 +787,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -864,25 +870,40 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1205,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662B42D0-2FDD-8740-B5DE-63A10E0A48C3}">
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1253,35 +1274,35 @@
       <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="13">
         <v>1</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="78" t="s">
+      <c r="C4" s="66"/>
+      <c r="D4" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78" t="s">
+      <c r="E4" s="56"/>
+      <c r="F4" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="78"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="5" t="s">
         <v>68</v>
       </c>
@@ -1294,1012 +1315,1039 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <v>2</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="84" t="s">
+      <c r="C5" s="66"/>
+      <c r="D5" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="78" t="s">
+      <c r="E5" s="64"/>
+      <c r="F5" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="86"/>
-      <c r="H5" s="79" t="s">
+      <c r="G5" s="57"/>
+      <c r="H5" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="80"/>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="80"/>
-      <c r="P5" s="80"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
     </row>
     <row r="6" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
         <v>3</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="84" t="s">
+      <c r="C6" s="66"/>
+      <c r="D6" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="85"/>
-      <c r="F6" s="78" t="s">
+      <c r="E6" s="64"/>
+      <c r="F6" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="86"/>
-      <c r="H6" s="79" t="s">
+      <c r="G6" s="57"/>
+      <c r="H6" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="80"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="81"/>
       <c r="Q6" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="121">
+    <row r="7" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="27">
         <v>4</v>
       </c>
-      <c r="B7" s="122" t="s">
+      <c r="B7" s="113" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="123"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="64"/>
+      <c r="F7" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="57"/>
+      <c r="H7" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="60"/>
     </row>
     <row r="8" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
+      <c r="A8" s="125">
+        <v>5</v>
+      </c>
+      <c r="B8" s="125" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="126"/>
+      <c r="D8" s="17"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="64"/>
-      <c r="C9" s="119"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+    </row>
+    <row r="12" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-    </row>
-    <row r="12" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:17" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="111" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="112"/>
+      <c r="H13" s="110" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="110"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="110"/>
+      <c r="N13" s="110"/>
+      <c r="O13" s="110"/>
+      <c r="P13" s="110"/>
+    </row>
+    <row r="14" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="117"/>
-      <c r="C13" s="118"/>
-      <c r="D13" s="113" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="114"/>
-      <c r="F13" s="114" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="114"/>
-      <c r="H13" s="112" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="112"/>
-      <c r="J13" s="112"/>
-      <c r="K13" s="112"/>
-      <c r="L13" s="112"/>
-      <c r="M13" s="112"/>
-      <c r="N13" s="112"/>
-      <c r="O13" s="112"/>
-      <c r="P13" s="112"/>
-    </row>
-    <row r="14" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
-        <v>1</v>
-      </c>
-      <c r="B14" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="8"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="79" t="s">
+      <c r="H14" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="80"/>
-      <c r="M14" s="80"/>
-      <c r="N14" s="80"/>
-      <c r="O14" s="80"/>
-      <c r="P14" s="97"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="81"/>
+      <c r="O14" s="81"/>
+      <c r="P14" s="95"/>
     </row>
     <row r="15" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A15" s="14">
+      <c r="A15" s="26">
+        <v>1</v>
+      </c>
+      <c r="B15" s="73" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="74"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13">
         <v>2</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B16" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-    </row>
-    <row r="16" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="115" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="115"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="78" t="s">
+      <c r="C16" s="66"/>
+      <c r="D16" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78" t="s">
+      <c r="E16" s="56"/>
+      <c r="F16" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="78"/>
+      <c r="G16" s="56"/>
       <c r="H16" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14">
+      <c r="A17" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="78"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="64"/>
+      <c r="F17" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="57"/>
+      <c r="H17" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="83"/>
+      <c r="O17" s="83"/>
+      <c r="P17" s="84"/>
+    </row>
+    <row r="18" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
         <v>1</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B18" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="63"/>
-      <c r="D17" s="84" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="85"/>
-      <c r="F17" s="78" t="s">
+      <c r="C18" s="66"/>
+      <c r="D18" s="93" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="94"/>
+      <c r="F18" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="86"/>
-      <c r="H17" s="81" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="82"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="82"/>
-      <c r="O17" s="82"/>
-      <c r="P17" s="83"/>
-    </row>
-    <row r="18" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14">
+      <c r="G18" s="101"/>
+      <c r="H18" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="81"/>
+      <c r="P18" s="95"/>
+    </row>
+    <row r="19" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
         <v>2</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B19" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="63"/>
-      <c r="D18" s="95" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="96"/>
-      <c r="F18" s="102" t="s">
+      <c r="C19" s="66"/>
+      <c r="D19" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="97"/>
+      <c r="F19" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="103"/>
-      <c r="H18" s="79" t="s">
-        <v>49</v>
-      </c>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
-      <c r="N18" s="80"/>
-      <c r="O18" s="80"/>
-      <c r="P18" s="97"/>
-    </row>
-    <row r="19" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+      <c r="G19" s="99"/>
+      <c r="H19" s="80" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
+      <c r="O19" s="81"/>
+      <c r="P19" s="95"/>
+    </row>
+    <row r="20" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
         <v>3</v>
       </c>
-      <c r="B19" s="62" t="s">
+      <c r="B20" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="98" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="99"/>
-      <c r="F19" s="100" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="101"/>
-      <c r="H19" s="79" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="80"/>
-      <c r="J19" s="80"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="80"/>
-      <c r="M19" s="80"/>
-      <c r="N19" s="80"/>
-      <c r="O19" s="80"/>
-      <c r="P19" s="97"/>
-    </row>
-    <row r="20" spans="1:16" ht="26" x14ac:dyDescent="0.2">
-      <c r="A20" s="28">
+      <c r="C20" s="66"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="27">
         <v>4</v>
       </c>
-      <c r="B20" s="62" t="s">
+      <c r="B21" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-    </row>
-    <row r="21" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="58" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="93" t="s">
+      <c r="C21" s="66"/>
+      <c r="D21" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93" t="s">
+      <c r="E21" s="91"/>
+      <c r="F21" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="93"/>
+      <c r="G21" s="91"/>
       <c r="H21" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="36">
+      <c r="A22" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="61"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="90"/>
+      <c r="F22" s="91" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="92"/>
+      <c r="H22" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="81"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="81"/>
+      <c r="N22" s="81"/>
+      <c r="O22" s="81"/>
+      <c r="P22" s="95"/>
+    </row>
+    <row r="23" spans="1:16" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="35">
         <v>1</v>
       </c>
-      <c r="B22" s="70" t="s">
+      <c r="B23" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="91" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="92"/>
-      <c r="F22" s="93" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="94"/>
-      <c r="H22" s="79" t="s">
-        <v>56</v>
-      </c>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="80"/>
-      <c r="L22" s="80"/>
-      <c r="M22" s="80"/>
-      <c r="N22" s="80"/>
-      <c r="O22" s="80"/>
-      <c r="P22" s="97"/>
-    </row>
-    <row r="23" spans="1:16" ht="38" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
-        <v>2</v>
-      </c>
-      <c r="B23" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="61"/>
-      <c r="D23" s="9"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="H23" s="79" t="s">
+      <c r="H23" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="80"/>
-      <c r="J23" s="80"/>
-      <c r="K23" s="80"/>
-      <c r="L23" s="80"/>
-      <c r="M23" s="80"/>
-      <c r="N23" s="80"/>
-      <c r="O23" s="80"/>
-      <c r="P23" s="97"/>
+      <c r="I23" s="81"/>
+      <c r="J23" s="81"/>
+      <c r="K23" s="81"/>
+      <c r="L23" s="81"/>
+      <c r="M23" s="81"/>
+      <c r="N23" s="81"/>
+      <c r="O23" s="81"/>
+      <c r="P23" s="95"/>
     </row>
     <row r="24" spans="1:16" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="30">
+      <c r="A24" s="28">
+        <v>2</v>
+      </c>
+      <c r="B24" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="74"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="81" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="81"/>
+      <c r="L24" s="81"/>
+      <c r="M24" s="81"/>
+      <c r="N24" s="81"/>
+      <c r="O24" s="81"/>
+      <c r="P24" s="95"/>
+    </row>
+    <row r="25" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
         <v>3</v>
       </c>
-      <c r="B24" s="62" t="s">
+      <c r="B25" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="63"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="80"/>
-      <c r="L24" s="80"/>
-      <c r="M24" s="80"/>
-      <c r="N24" s="80"/>
-      <c r="O24" s="80"/>
-      <c r="P24" s="97"/>
-    </row>
-    <row r="25" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="31">
+      <c r="C25" s="66"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+    </row>
+    <row r="26" spans="1:16" ht="19" x14ac:dyDescent="0.2">
+      <c r="A26" s="30">
         <v>4</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="B26" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="72"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-    </row>
-    <row r="26" spans="1:16" ht="26" x14ac:dyDescent="0.2">
-      <c r="A26" s="58" t="s">
+      <c r="C26" s="75"/>
+      <c r="D26" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="90"/>
+      <c r="F26" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="92"/>
+      <c r="H26" s="105" t="s">
+        <v>61</v>
+      </c>
+      <c r="I26" s="105"/>
+      <c r="J26" s="105"/>
+      <c r="K26" s="105"/>
+      <c r="L26" s="105"/>
+      <c r="M26" s="105"/>
+      <c r="N26" s="105"/>
+      <c r="O26" s="105"/>
+      <c r="P26" s="106"/>
+    </row>
+    <row r="27" spans="1:16" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="58"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="91" t="s">
+      <c r="B27" s="61"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="92"/>
-      <c r="F26" s="91" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="94"/>
-      <c r="H26" s="107" t="s">
-        <v>61</v>
-      </c>
-      <c r="I26" s="107"/>
-      <c r="J26" s="107"/>
-      <c r="K26" s="107"/>
-      <c r="L26" s="107"/>
-      <c r="M26" s="107"/>
-      <c r="N26" s="107"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="108"/>
-    </row>
-    <row r="27" spans="1:16" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="35">
-        <v>1</v>
-      </c>
-      <c r="B27" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="73"/>
-      <c r="D27" s="91" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="92"/>
-      <c r="F27" s="91" t="s">
+      <c r="E27" s="90"/>
+      <c r="F27" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="92"/>
-      <c r="H27" s="109" t="s">
+      <c r="G27" s="90"/>
+      <c r="H27" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="I27" s="110"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="110"/>
-      <c r="L27" s="110"/>
-      <c r="M27" s="110"/>
-      <c r="N27" s="110"/>
-      <c r="O27" s="110"/>
-      <c r="P27" s="111"/>
+      <c r="I27" s="108"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="108"/>
+      <c r="L27" s="108"/>
+      <c r="M27" s="108"/>
+      <c r="N27" s="108"/>
+      <c r="O27" s="108"/>
+      <c r="P27" s="109"/>
     </row>
     <row r="28" spans="1:16" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="34">
+        <v>1</v>
+      </c>
+      <c r="B28" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="117"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="102" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" s="103"/>
+      <c r="J28" s="103"/>
+      <c r="K28" s="103"/>
+      <c r="L28" s="103"/>
+      <c r="M28" s="103"/>
+      <c r="N28" s="103"/>
+      <c r="O28" s="103"/>
+      <c r="P28" s="104"/>
+    </row>
+    <row r="29" spans="1:16" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="33">
         <v>2</v>
       </c>
-      <c r="B28" s="72" t="s">
+      <c r="B29" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="73"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="104" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" s="105"/>
-      <c r="J28" s="105"/>
-      <c r="K28" s="105"/>
-      <c r="L28" s="105"/>
-      <c r="M28" s="105"/>
-      <c r="N28" s="105"/>
-      <c r="O28" s="105"/>
-      <c r="P28" s="106"/>
-    </row>
-    <row r="29" spans="1:16" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="54">
+      <c r="C29" s="117"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="54"/>
+    </row>
+    <row r="30" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="53">
         <v>3</v>
       </c>
-      <c r="B29" s="74" t="s">
+      <c r="B30" s="115" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="75"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="52"/>
-      <c r="N29" s="52"/>
-      <c r="O29" s="52"/>
-      <c r="P29" s="55"/>
-    </row>
-    <row r="30" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="37">
+      <c r="C30" s="116"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="48"/>
+      <c r="P30" s="46"/>
+    </row>
+    <row r="31" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" s="36">
         <v>4</v>
       </c>
-      <c r="B30" s="56" t="s">
+      <c r="B31" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="47"/>
-    </row>
-    <row r="31" spans="1:16" ht="26" x14ac:dyDescent="0.25">
-      <c r="A31" s="58" t="s">
+      <c r="C31" s="119"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+    </row>
+    <row r="32" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+      <c r="A32" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="58"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-    </row>
-    <row r="32" spans="1:16" ht="26" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
     </row>
     <row r="33" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-    </row>
-    <row r="34" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A34" s="58" t="s">
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+    </row>
+    <row r="34" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+    </row>
+    <row r="35" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+      <c r="A35" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
-    </row>
-    <row r="35" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
     </row>
     <row r="36" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-    </row>
-    <row r="37" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A37" s="58" t="s">
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
+    </row>
+    <row r="37" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+    </row>
+    <row r="38" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+      <c r="A38" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
-    </row>
-    <row r="38" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
     </row>
     <row r="39" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="40"/>
-      <c r="J39" s="40"/>
-    </row>
-    <row r="40" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A40" s="58" t="s">
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+    </row>
+    <row r="40" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+    </row>
+    <row r="41" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+      <c r="A41" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="58"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="40"/>
-      <c r="J40" s="40"/>
-    </row>
-    <row r="41" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A41" s="19">
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="41"/>
+      <c r="I41" s="41"/>
+      <c r="J41" s="41"/>
+    </row>
+    <row r="42" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="18">
         <v>1</v>
       </c>
-      <c r="B41" s="68" t="s">
+      <c r="B42" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
-    </row>
-    <row r="42" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
-    </row>
-    <row r="43" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A43" s="58" t="s">
+      <c r="C42" s="124"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
+    </row>
+    <row r="43" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
+    </row>
+    <row r="44" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+      <c r="A44" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="58"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
-    </row>
-    <row r="44" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
-    </row>
-    <row r="45" spans="1:17" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
+    </row>
+    <row r="45" spans="1:17" s="22" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="87" t="s">
+      <c r="D45" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="88"/>
-      <c r="F45" s="89" t="s">
+      <c r="E45" s="86"/>
+      <c r="F45" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="G45" s="90"/>
-      <c r="H45" s="24" t="s">
+      <c r="G45" s="88"/>
+      <c r="H45" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="Q45" s="24"/>
-    </row>
-    <row r="46" spans="1:17" s="23" customFormat="1" ht="26" x14ac:dyDescent="0.25">
-      <c r="A46" s="58" t="s">
+      <c r="Q45" s="23"/>
+    </row>
+    <row r="46" spans="1:17" s="22" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="85" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="86"/>
+      <c r="F46" s="86" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="88"/>
+      <c r="H46" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q46" s="23"/>
+    </row>
+    <row r="47" spans="1:17" s="22" customFormat="1" ht="26" x14ac:dyDescent="0.25">
+      <c r="A47" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="58"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="88"/>
-      <c r="F46" s="88" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="90"/>
-      <c r="H46" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q46" s="24"/>
-    </row>
-    <row r="47" spans="1:17" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A47" s="20">
+      <c r="B47" s="61"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="50"/>
+      <c r="Q47" s="23"/>
+    </row>
+    <row r="48" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+      <c r="A48" s="19">
         <v>1</v>
       </c>
-      <c r="B47" s="65" t="s">
+      <c r="B48" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="66"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="51"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="51"/>
-      <c r="K47" s="51"/>
-      <c r="Q47" s="24"/>
-    </row>
-    <row r="48" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A48" s="25">
+      <c r="C48" s="121"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="41"/>
+      <c r="H48" s="41"/>
+      <c r="I48" s="41"/>
+      <c r="J48" s="41"/>
+      <c r="K48" s="39"/>
+    </row>
+    <row r="49" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A49" s="24">
         <v>2</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B49" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="26"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="40"/>
-    </row>
-    <row r="49" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A49" s="22">
+      <c r="C49" s="25"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="39"/>
+    </row>
+    <row r="50" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A50" s="21">
         <v>3</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B50" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="21"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="40"/>
-      <c r="J49" s="40"/>
-      <c r="K49" s="40"/>
-    </row>
-    <row r="50" spans="1:11" ht="26" x14ac:dyDescent="0.25">
-      <c r="A50" s="58" t="s">
+      <c r="C50" s="20"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="39"/>
+    </row>
+    <row r="51" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A51" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="58"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="40"/>
-      <c r="J50" s="40"/>
-      <c r="K50" s="40"/>
-    </row>
-    <row r="51" spans="1:11" ht="26" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="42"/>
-      <c r="K51" s="40"/>
+      <c r="B51" s="61"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="41"/>
+      <c r="K51" s="39"/>
     </row>
     <row r="52" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="40"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="40"/>
-      <c r="J52" s="40"/>
-      <c r="K52" s="40"/>
-    </row>
-    <row r="53" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A53" s="58" t="s">
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="39"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="39"/>
+    </row>
+    <row r="53" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="39"/>
+      <c r="J53" s="39"/>
+      <c r="K53" s="39"/>
+    </row>
+    <row r="54" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A54" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="58"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="40"/>
-      <c r="J53" s="40"/>
-      <c r="K53" s="40"/>
-    </row>
-    <row r="54" spans="1:11" ht="26" x14ac:dyDescent="0.25">
-      <c r="A54" s="21">
+      <c r="B54" s="61"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="41"/>
+      <c r="I54" s="41"/>
+      <c r="J54" s="41"/>
+      <c r="K54" s="39"/>
+    </row>
+    <row r="55" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A55" s="20">
         <v>1</v>
       </c>
-      <c r="B54" s="65" t="s">
+      <c r="B55" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="67"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="42"/>
-      <c r="J54" s="42"/>
-      <c r="K54" s="40"/>
-    </row>
-    <row r="55" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="40"/>
-      <c r="K55" s="40"/>
-    </row>
-    <row r="56" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A56" s="58" t="s">
+      <c r="C55" s="122"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="39"/>
+    </row>
+    <row r="56" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="39"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="39"/>
+    </row>
+    <row r="57" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A57" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="B56" s="58"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="40"/>
-      <c r="J56" s="40"/>
-      <c r="K56" s="40"/>
-    </row>
-    <row r="57" spans="1:11" ht="26" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="42"/>
-      <c r="F57" s="42"/>
-      <c r="G57" s="42"/>
-      <c r="H57" s="42"/>
-      <c r="I57" s="42"/>
-      <c r="J57" s="42"/>
-      <c r="K57" s="40"/>
+      <c r="B57" s="61"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="41"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="41"/>
+      <c r="G57" s="41"/>
+      <c r="H57" s="41"/>
+      <c r="I57" s="41"/>
+      <c r="J57" s="41"/>
+      <c r="K57" s="39"/>
     </row>
     <row r="58" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="40"/>
-      <c r="K58" s="40"/>
-    </row>
-    <row r="59" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A59" s="58" t="s">
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="39"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="39"/>
+    </row>
+    <row r="59" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="39"/>
+      <c r="I59" s="39"/>
+      <c r="J59" s="39"/>
+      <c r="K59" s="39"/>
+    </row>
+    <row r="60" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A60" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="B59" s="58"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="40"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="40"/>
-      <c r="I59" s="40"/>
-      <c r="J59" s="40"/>
-      <c r="K59" s="40"/>
-    </row>
-    <row r="60" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="D60" s="42"/>
-      <c r="E60" s="42"/>
-      <c r="F60" s="42"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="42"/>
-      <c r="I60" s="42"/>
-      <c r="J60" s="42"/>
-    </row>
-    <row r="62" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A62" s="58" t="s">
+      <c r="B60" s="61"/>
+      <c r="C60" s="61"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="41"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="41"/>
+      <c r="I60" s="41"/>
+      <c r="J60" s="41"/>
+    </row>
+    <row r="63" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A63" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="58"/>
-      <c r="C62" s="59"/>
-    </row>
-    <row r="63" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="62"/>
     </row>
     <row r="64" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
+    <row r="65" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="84">
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A11:C11"/>
+  <mergeCells count="87">
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A12:C12"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A51:C51"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H13:P13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="H14:P14"/>
-    <mergeCell ref="H22:P22"/>
-    <mergeCell ref="H23:P23"/>
-    <mergeCell ref="H24:P24"/>
-    <mergeCell ref="H28:P28"/>
-    <mergeCell ref="H26:P26"/>
-    <mergeCell ref="H27:P27"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="D18:E18"/>
@@ -2308,6 +2356,53 @@
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H22:P22"/>
+    <mergeCell ref="H23:P23"/>
+    <mergeCell ref="H24:P24"/>
+    <mergeCell ref="H28:P28"/>
+    <mergeCell ref="H26:P26"/>
+    <mergeCell ref="H27:P27"/>
+    <mergeCell ref="H6:P6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H1:J2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="H5:P5"/>
+    <mergeCell ref="H17:P17"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:P7"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="F46:G46"/>
@@ -2317,56 +2412,6 @@
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="H6:P6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="H1:J2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H5:P5"/>
-    <mergeCell ref="H17:P17"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
longest rep. char replacement done
</commit_message>
<xml_diff>
--- a/neetcode_150/neetcode150_fast_reviews.xlsx
+++ b/neetcode_150/neetcode150_fast_reviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mys1erious/Desktop/StudyProgramming/Git/algorithms/neetcode_150/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DD4701-9F03-7D43-832C-A6BA30BE5AB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2E7781-CB2A-CE45-A841-BFC0549DD2EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="920" windowWidth="28040" windowHeight="17440" xr2:uid="{76CD3ECE-D592-4947-8368-191EE7B52C35}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="88">
   <si>
     <t>Arrays and Hashing</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>if s[rp] in set, remove s[lp] until s[rp] in set, otherwise add s[rp] to set</t>
+  </si>
+  <si>
+    <t>Longest Repeating Char Replacement</t>
+  </si>
+  <si>
+    <t>maintain 'most occurred char' and 'sum of all chars'; if 'sum of all chars' - 'most occurred char' &gt; k, then u need to shift 'lp', decrease its value in counts and decrease 'sum of all chars' until its false, otherwise u just shift rp and increase sum of all chars</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -694,23 +700,200 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -718,27 +901,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -775,166 +937,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1251,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662B42D0-2FDD-8740-B5DE-63A10E0A48C3}">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1267,54 +1276,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="127"/>
+      <c r="B1" s="91"/>
       <c r="C1" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="128" t="s">
+      <c r="D1" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="128"/>
-      <c r="F1" s="129" t="s">
+      <c r="E1" s="92"/>
+      <c r="F1" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="129"/>
+      <c r="G1" s="93"/>
       <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="120" t="s">
+      <c r="C2" s="70"/>
+      <c r="D2" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="124" t="s">
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="124"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
       <c r="K3" s="47"/>
       <c r="L3" s="47"/>
       <c r="M3" s="47"/>
@@ -1323,11 +1332,11 @@
       <c r="P3" s="48"/>
     </row>
     <row r="4" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="121"/>
-      <c r="C4" s="121"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -1340,18 +1349,18 @@
       <c r="A5" s="9">
         <v>1</v>
       </c>
-      <c r="B5" s="116" t="s">
+      <c r="B5" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="117"/>
-      <c r="D5" s="118" t="s">
+      <c r="C5" s="108"/>
+      <c r="D5" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118" t="s">
+      <c r="E5" s="106"/>
+      <c r="F5" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="118"/>
+      <c r="G5" s="106"/>
       <c r="H5" s="4" t="s">
         <v>47</v>
       </c>
@@ -1367,57 +1376,57 @@
       <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="116" t="s">
+      <c r="B6" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="117"/>
-      <c r="D6" s="99" t="s">
+      <c r="C6" s="108"/>
+      <c r="D6" s="115" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="118" t="s">
+      <c r="E6" s="94"/>
+      <c r="F6" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="119"/>
-      <c r="H6" s="114" t="s">
+      <c r="G6" s="116"/>
+      <c r="H6" s="113" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="115"/>
-      <c r="O6" s="115"/>
-      <c r="P6" s="115"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="114"/>
+      <c r="M6" s="114"/>
+      <c r="N6" s="114"/>
+      <c r="O6" s="114"/>
+      <c r="P6" s="114"/>
     </row>
     <row r="7" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="116" t="s">
+      <c r="B7" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="117"/>
-      <c r="D7" s="99" t="s">
+      <c r="C7" s="108"/>
+      <c r="D7" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="98"/>
-      <c r="F7" s="118" t="s">
+      <c r="E7" s="94"/>
+      <c r="F7" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="119"/>
-      <c r="H7" s="114" t="s">
+      <c r="G7" s="116"/>
+      <c r="H7" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="115"/>
-      <c r="J7" s="115"/>
-      <c r="K7" s="115"/>
-      <c r="L7" s="115"/>
-      <c r="M7" s="115"/>
-      <c r="N7" s="115"/>
-      <c r="O7" s="115"/>
-      <c r="P7" s="115"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="114"/>
+      <c r="L7" s="114"/>
+      <c r="M7" s="114"/>
+      <c r="N7" s="114"/>
+      <c r="O7" s="114"/>
+      <c r="P7" s="114"/>
       <c r="Q7" s="5" t="s">
         <v>35</v>
       </c>
@@ -1426,29 +1435,29 @@
       <c r="A8" s="15">
         <v>4</v>
       </c>
-      <c r="B8" s="135" t="s">
+      <c r="B8" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="136"/>
-      <c r="D8" s="99" t="s">
+      <c r="C8" s="76"/>
+      <c r="D8" s="115" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="98"/>
-      <c r="F8" s="118" t="s">
+      <c r="E8" s="94"/>
+      <c r="F8" s="106" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="119"/>
-      <c r="H8" s="76" t="s">
+      <c r="G8" s="116"/>
+      <c r="H8" s="117" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="77"/>
-      <c r="P8" s="78"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="118"/>
+      <c r="N8" s="118"/>
+      <c r="O8" s="118"/>
+      <c r="P8" s="119"/>
     </row>
     <row r="9" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -1458,53 +1467,53 @@
         <v>56</v>
       </c>
       <c r="C9" s="37"/>
-      <c r="D9" s="99" t="s">
+      <c r="D9" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="98"/>
-      <c r="F9" s="126" t="s">
+      <c r="E9" s="94"/>
+      <c r="F9" s="112" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="96"/>
-      <c r="H9" s="91" t="s">
+      <c r="G9" s="90"/>
+      <c r="H9" s="122" t="s">
         <v>57</v>
       </c>
-      <c r="I9" s="92"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92"/>
-      <c r="L9" s="92"/>
-      <c r="M9" s="92"/>
-      <c r="N9" s="92"/>
-      <c r="O9" s="92"/>
-      <c r="P9" s="93"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="120"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="120"/>
+      <c r="O9" s="120"/>
+      <c r="P9" s="121"/>
     </row>
     <row r="10" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="36">
         <v>6</v>
       </c>
-      <c r="B10" s="116" t="s">
+      <c r="B10" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="116"/>
-      <c r="D10" s="94" t="s">
+      <c r="C10" s="107"/>
+      <c r="D10" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95" t="s">
+      <c r="E10" s="89"/>
+      <c r="F10" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="96"/>
-      <c r="H10" s="92" t="s">
+      <c r="G10" s="90"/>
+      <c r="H10" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="92"/>
-      <c r="M10" s="92"/>
-      <c r="N10" s="92"/>
-      <c r="O10" s="92"/>
-      <c r="P10" s="93"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="M10" s="120"/>
+      <c r="N10" s="120"/>
+      <c r="O10" s="120"/>
+      <c r="P10" s="121"/>
     </row>
     <row r="11" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="39">
@@ -1514,49 +1523,49 @@
         <v>60</v>
       </c>
       <c r="C11" s="39"/>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101" t="s">
+      <c r="E11" s="110"/>
+      <c r="F11" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="125"/>
-      <c r="H11" s="92" t="s">
+      <c r="G11" s="111"/>
+      <c r="H11" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="92"/>
-      <c r="O11" s="92"/>
-      <c r="P11" s="93"/>
+      <c r="I11" s="120"/>
+      <c r="J11" s="120"/>
+      <c r="K11" s="120"/>
+      <c r="L11" s="120"/>
+      <c r="M11" s="120"/>
+      <c r="N11" s="120"/>
+      <c r="O11" s="120"/>
+      <c r="P11" s="121"/>
     </row>
     <row r="12" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="46">
         <v>8</v>
       </c>
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="143"/>
+      <c r="C12" s="86"/>
       <c r="D12" s="10"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="82" t="s">
+      <c r="H12" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="83"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="83"/>
-      <c r="M12" s="83"/>
-      <c r="N12" s="83"/>
-      <c r="O12" s="83"/>
-      <c r="P12" s="84"/>
+      <c r="I12" s="135"/>
+      <c r="J12" s="135"/>
+      <c r="K12" s="135"/>
+      <c r="L12" s="135"/>
+      <c r="M12" s="135"/>
+      <c r="N12" s="135"/>
+      <c r="O12" s="135"/>
+      <c r="P12" s="136"/>
     </row>
     <row r="13" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="56">
@@ -1566,32 +1575,32 @@
         <v>68</v>
       </c>
       <c r="C13" s="57"/>
-      <c r="D13" s="85" t="s">
+      <c r="D13" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86" t="s">
+      <c r="E13" s="138"/>
+      <c r="F13" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="87"/>
-      <c r="H13" s="79" t="s">
+      <c r="G13" s="139"/>
+      <c r="H13" s="131" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="81"/>
+      <c r="I13" s="132"/>
+      <c r="J13" s="132"/>
+      <c r="K13" s="132"/>
+      <c r="L13" s="132"/>
+      <c r="M13" s="132"/>
+      <c r="N13" s="132"/>
+      <c r="O13" s="132"/>
+      <c r="P13" s="133"/>
     </row>
     <row r="14" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="121"/>
-      <c r="C14" s="131"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="74"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1611,58 +1620,58 @@
       <c r="A15" s="61">
         <v>1</v>
       </c>
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="126" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="107"/>
-      <c r="D15" s="74" t="s">
+      <c r="C15" s="127"/>
+      <c r="D15" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74" t="s">
+      <c r="E15" s="95"/>
+      <c r="F15" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="74"/>
-      <c r="H15" s="76" t="s">
+      <c r="G15" s="95"/>
+      <c r="H15" s="117" t="s">
         <v>73</v>
       </c>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="77"/>
-      <c r="N15" s="77"/>
-      <c r="O15" s="77"/>
-      <c r="P15" s="78"/>
+      <c r="I15" s="118"/>
+      <c r="J15" s="118"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="118"/>
+      <c r="N15" s="118"/>
+      <c r="O15" s="118"/>
+      <c r="P15" s="119"/>
       <c r="Q15" s="18"/>
     </row>
     <row r="16" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="63">
         <v>2</v>
       </c>
-      <c r="B16" s="106" t="s">
+      <c r="B16" s="126" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="107"/>
-      <c r="D16" s="73" t="s">
+      <c r="C16" s="127"/>
+      <c r="D16" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74" t="s">
+      <c r="E16" s="95"/>
+      <c r="F16" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="75"/>
-      <c r="H16" s="76" t="s">
+      <c r="G16" s="102"/>
+      <c r="H16" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="77"/>
-      <c r="J16" s="77"/>
-      <c r="K16" s="77"/>
-      <c r="L16" s="77"/>
-      <c r="M16" s="77"/>
-      <c r="N16" s="77"/>
-      <c r="O16" s="77"/>
-      <c r="P16" s="78"/>
+      <c r="I16" s="118"/>
+      <c r="J16" s="118"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="118"/>
+      <c r="M16" s="118"/>
+      <c r="N16" s="118"/>
+      <c r="O16" s="118"/>
+      <c r="P16" s="119"/>
       <c r="Q16" s="18"/>
     </row>
     <row r="17" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -1673,25 +1682,25 @@
         <v>75</v>
       </c>
       <c r="C17" s="59"/>
-      <c r="D17" s="73" t="s">
+      <c r="D17" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74" t="s">
+      <c r="E17" s="95"/>
+      <c r="F17" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="75"/>
-      <c r="H17" s="76" t="s">
+      <c r="G17" s="102"/>
+      <c r="H17" s="117" t="s">
         <v>76</v>
       </c>
-      <c r="I17" s="77"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="77"/>
-      <c r="L17" s="77"/>
-      <c r="M17" s="77"/>
-      <c r="N17" s="77"/>
-      <c r="O17" s="77"/>
-      <c r="P17" s="78"/>
+      <c r="I17" s="118"/>
+      <c r="J17" s="118"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="118"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="118"/>
+      <c r="O17" s="118"/>
+      <c r="P17" s="119"/>
       <c r="Q17" s="18"/>
     </row>
     <row r="18" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -1702,58 +1711,58 @@
         <v>77</v>
       </c>
       <c r="C18" s="59"/>
-      <c r="D18" s="73" t="s">
+      <c r="D18" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74" t="s">
+      <c r="E18" s="95"/>
+      <c r="F18" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="75"/>
-      <c r="H18" s="76" t="s">
+      <c r="G18" s="102"/>
+      <c r="H18" s="117" t="s">
         <v>78</v>
       </c>
-      <c r="I18" s="77"/>
-      <c r="J18" s="77"/>
-      <c r="K18" s="77"/>
-      <c r="L18" s="77"/>
-      <c r="M18" s="77"/>
-      <c r="N18" s="77"/>
-      <c r="O18" s="77"/>
-      <c r="P18" s="78"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="118"/>
+      <c r="L18" s="118"/>
+      <c r="M18" s="118"/>
+      <c r="N18" s="118"/>
+      <c r="O18" s="118"/>
+      <c r="P18" s="119"/>
       <c r="Q18" s="18"/>
     </row>
     <row r="19" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="62">
         <v>5</v>
       </c>
-      <c r="B19" s="67" t="s">
+      <c r="B19" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="68"/>
+      <c r="C19" s="65"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
       <c r="G19" s="60"/>
-      <c r="H19" s="88" t="s">
+      <c r="H19" s="140" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="89"/>
-      <c r="J19" s="89"/>
-      <c r="K19" s="89"/>
-      <c r="L19" s="89"/>
-      <c r="M19" s="89"/>
-      <c r="N19" s="89"/>
-      <c r="O19" s="89"/>
-      <c r="P19" s="90"/>
+      <c r="I19" s="141"/>
+      <c r="J19" s="141"/>
+      <c r="K19" s="141"/>
+      <c r="L19" s="141"/>
+      <c r="M19" s="141"/>
+      <c r="N19" s="141"/>
+      <c r="O19" s="141"/>
+      <c r="P19" s="142"/>
       <c r="Q19" s="18"/>
     </row>
     <row r="20" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="121" t="s">
+      <c r="A20" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="121"/>
-      <c r="C20" s="131"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="74"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
       <c r="F20" s="40"/>
@@ -1770,139 +1779,147 @@
       <c r="Q20" s="18"/>
     </row>
     <row r="21" spans="1:17" ht="19" x14ac:dyDescent="0.2">
-      <c r="A21" s="64">
+      <c r="A21" s="66">
         <v>1</v>
       </c>
-      <c r="B21" s="110" t="s">
+      <c r="B21" s="126" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="111"/>
-      <c r="D21" s="94" t="s">
+      <c r="C21" s="127"/>
+      <c r="D21" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="95"/>
-      <c r="F21" s="95" t="s">
+      <c r="E21" s="89"/>
+      <c r="F21" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="96"/>
-      <c r="H21" s="91" t="s">
+      <c r="G21" s="90"/>
+      <c r="H21" s="122" t="s">
         <v>83</v>
       </c>
-      <c r="I21" s="92"/>
-      <c r="J21" s="92"/>
-      <c r="K21" s="92"/>
-      <c r="L21" s="92"/>
-      <c r="M21" s="92"/>
-      <c r="N21" s="92"/>
-      <c r="O21" s="92"/>
-      <c r="P21" s="93"/>
+      <c r="I21" s="120"/>
+      <c r="J21" s="120"/>
+      <c r="K21" s="120"/>
+      <c r="L21" s="120"/>
+      <c r="M21" s="120"/>
+      <c r="N21" s="120"/>
+      <c r="O21" s="120"/>
+      <c r="P21" s="121"/>
       <c r="Q21" s="18"/>
     </row>
     <row r="22" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="66">
+      <c r="A22" s="68">
         <v>2</v>
       </c>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="94" t="s">
+      <c r="C22" s="67"/>
+      <c r="D22" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="95"/>
-      <c r="F22" s="95" t="s">
+      <c r="E22" s="89"/>
+      <c r="F22" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="96"/>
-      <c r="H22" s="91" t="s">
+      <c r="G22" s="90"/>
+      <c r="H22" s="122" t="s">
         <v>85</v>
       </c>
-      <c r="I22" s="92"/>
-      <c r="J22" s="92"/>
-      <c r="K22" s="92"/>
-      <c r="L22" s="92"/>
-      <c r="M22" s="92"/>
-      <c r="N22" s="92"/>
-      <c r="O22" s="92"/>
-      <c r="P22" s="93"/>
+      <c r="I22" s="120"/>
+      <c r="J22" s="120"/>
+      <c r="K22" s="120"/>
+      <c r="L22" s="120"/>
+      <c r="M22" s="120"/>
+      <c r="N22" s="120"/>
+      <c r="O22" s="120"/>
+      <c r="P22" s="121"/>
       <c r="Q22" s="18"/>
     </row>
-    <row r="23" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="132" t="s">
+    <row r="23" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="69">
+        <v>3</v>
+      </c>
+      <c r="B23" s="144" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="145"/>
+      <c r="D23" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="90"/>
+      <c r="H23" s="122" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="120"/>
+      <c r="J23" s="120"/>
+      <c r="K23" s="120"/>
+      <c r="L23" s="120"/>
+      <c r="M23" s="120"/>
+      <c r="N23" s="120"/>
+      <c r="O23" s="120"/>
+      <c r="P23" s="121"/>
+      <c r="Q23" s="18"/>
+    </row>
+    <row r="24" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="132"/>
-      <c r="C23" s="133"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98"/>
-      <c r="G23" s="98"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="18"/>
-    </row>
-    <row r="24" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="26">
+      <c r="B24" s="97"/>
+      <c r="C24" s="98"/>
+      <c r="D24" s="94"/>
+      <c r="E24" s="94"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="94"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="18"/>
+    </row>
+    <row r="25" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="26">
         <v>1</v>
       </c>
-      <c r="B24" s="112" t="s">
+      <c r="B25" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="134"/>
-      <c r="D24" s="98"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="98"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="55"/>
-      <c r="Q24" s="18"/>
-    </row>
-    <row r="25" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27">
+      <c r="C25" s="100"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="94"/>
+      <c r="G25" s="94"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="18"/>
+    </row>
+    <row r="26" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="27">
         <v>2</v>
       </c>
-      <c r="B25" s="108" t="s">
+      <c r="B26" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="109"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="53"/>
-      <c r="Q25" s="18"/>
-    </row>
-    <row r="26" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="122" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="122"/>
-      <c r="C26" s="123"/>
-      <c r="D26" s="130"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="130"/>
-      <c r="G26" s="130"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
       <c r="H26" s="50"/>
       <c r="I26" s="41"/>
       <c r="J26" s="41"/>
@@ -1914,43 +1931,42 @@
       <c r="P26" s="53"/>
       <c r="Q26" s="18"/>
     </row>
-    <row r="27" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A27" s="27">
+    <row r="27" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="104" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="104"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="96"/>
+      <c r="G27" s="96"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="18"/>
+    </row>
+    <row r="28" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+      <c r="A28" s="27">
         <v>1</v>
       </c>
-      <c r="B27" s="108" t="s">
+      <c r="B28" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="109"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="54"/>
-      <c r="Q27" s="18"/>
-    </row>
-    <row r="28" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27">
-        <v>2</v>
-      </c>
-      <c r="B28" s="108" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="109"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="72"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
       <c r="K28" s="18"/>
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
@@ -1959,41 +1975,40 @@
       <c r="P28" s="54"/>
       <c r="Q28" s="18"/>
     </row>
-    <row r="29" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27">
+        <v>2</v>
+      </c>
+      <c r="B29" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="78"/>
+      <c r="D29" s="109"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="109"/>
+      <c r="G29" s="109"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="54"/>
+      <c r="Q29" s="18"/>
+    </row>
+    <row r="30" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="27">
         <v>3</v>
       </c>
-      <c r="B29" s="108" t="s">
+      <c r="B30" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="109"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="53"/>
-      <c r="Q29" s="18"/>
-    </row>
-    <row r="30" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25">
-        <v>4</v>
-      </c>
-      <c r="B30" s="108" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="109"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="109"/>
+      <c r="E30" s="109"/>
+      <c r="F30" s="109"/>
+      <c r="G30" s="109"/>
       <c r="H30" s="50"/>
       <c r="I30" s="41"/>
       <c r="J30" s="41"/>
@@ -2005,16 +2020,18 @@
       <c r="P30" s="53"/>
       <c r="Q30" s="18"/>
     </row>
-    <row r="31" spans="1:17" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="104" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="104"/>
-      <c r="C31" s="105"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
+    <row r="31" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25">
+        <v>4</v>
+      </c>
+      <c r="B31" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="78"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="18"/>
       <c r="H31" s="50"/>
       <c r="I31" s="41"/>
       <c r="J31" s="41"/>
@@ -2026,150 +2043,148 @@
       <c r="P31" s="53"/>
       <c r="Q31" s="18"/>
     </row>
-    <row r="32" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A32" s="28">
+    <row r="32" spans="1:17" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="71"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="53"/>
+      <c r="Q32" s="18"/>
+    </row>
+    <row r="33" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="28">
         <v>1</v>
       </c>
-      <c r="B32" s="144" t="s">
+      <c r="B33" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="144"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-    </row>
-    <row r="33" spans="1:17" ht="19" x14ac:dyDescent="0.2">
-      <c r="A33" s="29">
+      <c r="C33" s="87"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+    </row>
+    <row r="34" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A34" s="29">
         <v>2</v>
       </c>
-      <c r="B33" s="112" t="s">
+      <c r="B34" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="112"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="43"/>
-      <c r="P33" s="43"/>
-      <c r="Q33" s="18"/>
-    </row>
-    <row r="34" spans="1:17" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="30">
+      <c r="C34" s="99"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="43"/>
+      <c r="P34" s="43"/>
+      <c r="Q34" s="18"/>
+    </row>
+    <row r="35" spans="1:17" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="30">
         <v>3</v>
       </c>
-      <c r="B34" s="108" t="s">
+      <c r="B35" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="108"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="44"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="44"/>
-      <c r="N34" s="44"/>
-      <c r="O34" s="44"/>
-      <c r="P34" s="44"/>
-      <c r="Q34" s="18"/>
-    </row>
-    <row r="35" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="31">
+      <c r="C35" s="77"/>
+      <c r="D35" s="109"/>
+      <c r="E35" s="109"/>
+      <c r="F35" s="109"/>
+      <c r="G35" s="109"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="44"/>
+      <c r="P35" s="44"/>
+      <c r="Q35" s="18"/>
+    </row>
+    <row r="36" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="31">
         <v>4</v>
       </c>
-      <c r="B35" s="110" t="s">
+      <c r="B36" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="110"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42"/>
-      <c r="K35" s="42"/>
-      <c r="L35" s="42"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="42"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="42"/>
-      <c r="Q35" s="18"/>
-    </row>
-    <row r="36" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="104" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="104"/>
-      <c r="C36" s="104"/>
+      <c r="C36" s="79"/>
       <c r="D36" s="38"/>
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="24"/>
-      <c r="O36" s="24"/>
-      <c r="P36" s="24"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="42"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="42"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="42"/>
       <c r="Q36" s="18"/>
     </row>
-    <row r="37" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A37" s="31">
+    <row r="37" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="18"/>
+    </row>
+    <row r="38" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A38" s="31">
         <v>1</v>
       </c>
-      <c r="B37" s="110" t="s">
+      <c r="B38" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="110"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-    </row>
-    <row r="38" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A38" s="30">
-        <v>2</v>
-      </c>
-      <c r="B38" s="110" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="110"/>
+      <c r="C38" s="79"/>
       <c r="D38" s="21"/>
       <c r="E38" s="21"/>
       <c r="F38" s="21"/>
@@ -2185,44 +2200,53 @@
       <c r="P38" s="18"/>
       <c r="Q38" s="18"/>
     </row>
-    <row r="39" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A39" s="32">
+    <row r="39" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="30">
+        <v>2</v>
+      </c>
+      <c r="B39" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="79"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+    </row>
+    <row r="40" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+      <c r="A40" s="32">
         <v>3</v>
       </c>
-      <c r="B39" s="108" t="s">
+      <c r="B40" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="109"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-    </row>
-    <row r="40" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
+      <c r="C40" s="78"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="17">
         <v>4</v>
       </c>
-      <c r="B40" s="137" t="s">
+      <c r="B41" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="138"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-    </row>
-    <row r="41" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A41" s="104" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="104"/>
-      <c r="C41" s="105"/>
+      <c r="C41" s="81"/>
       <c r="D41" s="21"/>
       <c r="E41" s="21"/>
       <c r="F41" s="21"/>
@@ -2231,36 +2255,36 @@
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
     </row>
-    <row r="42" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-    </row>
-    <row r="43" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A42" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="71"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+    </row>
+    <row r="43" spans="1:17" ht="26" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-    </row>
-    <row r="44" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A44" s="104" t="s">
-        <v>18</v>
-      </c>
-      <c r="B44" s="104"/>
-      <c r="C44" s="104"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
       <c r="D44" s="21"/>
       <c r="E44" s="21"/>
       <c r="F44" s="21"/>
@@ -2269,36 +2293,36 @@
       <c r="I44" s="18"/>
       <c r="J44" s="18"/>
     </row>
-    <row r="45" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-    </row>
-    <row r="46" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A45" s="71" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="71"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+    </row>
+    <row r="46" spans="1:17" ht="26" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-    </row>
-    <row r="47" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A47" s="104" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="104"/>
-      <c r="C47" s="104"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+    </row>
+    <row r="47" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
       <c r="D47" s="21"/>
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
@@ -2307,36 +2331,36 @@
       <c r="I47" s="18"/>
       <c r="J47" s="18"/>
     </row>
-    <row r="48" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-    </row>
-    <row r="49" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A48" s="71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="71"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+    </row>
+    <row r="49" spans="1:17" ht="26" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-    </row>
-    <row r="50" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A50" s="104" t="s">
-        <v>20</v>
-      </c>
-      <c r="B50" s="104"/>
-      <c r="C50" s="104"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+    </row>
+    <row r="50" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
       <c r="D50" s="21"/>
       <c r="E50" s="21"/>
       <c r="F50" s="21"/>
@@ -2345,96 +2369,93 @@
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
     </row>
-    <row r="51" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A51" s="12">
+    <row r="51" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A51" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="71"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+    </row>
+    <row r="52" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+      <c r="A52" s="12">
         <v>1</v>
       </c>
-      <c r="B51" s="102" t="s">
+      <c r="B52" s="124" t="s">
         <v>33</v>
       </c>
-      <c r="C51" s="103"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-    </row>
-    <row r="52" spans="1:17" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="97"/>
-      <c r="E52" s="70"/>
-      <c r="F52" s="113"/>
-      <c r="G52" s="71"/>
-      <c r="H52" s="14"/>
-      <c r="Q52" s="14"/>
-    </row>
-    <row r="53" spans="1:17" s="13" customFormat="1" ht="26" x14ac:dyDescent="0.25">
-      <c r="A53" s="104" t="s">
-        <v>21</v>
-      </c>
-      <c r="B53" s="104"/>
-      <c r="C53" s="104"/>
-      <c r="D53" s="97"/>
-      <c r="E53" s="70"/>
-      <c r="F53" s="70"/>
-      <c r="G53" s="71"/>
+      <c r="C52" s="125"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+    </row>
+    <row r="53" spans="1:17" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="128"/>
+      <c r="E53" s="129"/>
+      <c r="F53" s="143"/>
+      <c r="G53" s="130"/>
       <c r="H53" s="14"/>
       <c r="Q53" s="14"/>
     </row>
-    <row r="54" spans="1:17" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="23"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="23"/>
-      <c r="K54" s="23"/>
+    <row r="54" spans="1:17" s="13" customFormat="1" ht="26" x14ac:dyDescent="0.25">
+      <c r="A54" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="71"/>
+      <c r="C54" s="71"/>
+      <c r="D54" s="128"/>
+      <c r="E54" s="129"/>
+      <c r="F54" s="129"/>
+      <c r="G54" s="130"/>
+      <c r="H54" s="14"/>
       <c r="Q54" s="14"/>
     </row>
-    <row r="55" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="18"/>
-    </row>
-    <row r="56" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A56" s="104" t="s">
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="23"/>
+      <c r="K55" s="23"/>
+      <c r="Q55" s="14"/>
+    </row>
+    <row r="56" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="18"/>
+    </row>
+    <row r="57" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A57" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B56" s="104"/>
-      <c r="C56" s="105"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
-    </row>
-    <row r="57" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A57" s="32">
-        <v>1</v>
-      </c>
-      <c r="B57" s="139" t="s">
-        <v>31</v>
-      </c>
-      <c r="C57" s="140"/>
+      <c r="B57" s="71"/>
+      <c r="C57" s="72"/>
       <c r="D57" s="21"/>
       <c r="E57" s="21"/>
       <c r="F57" s="21"/>
@@ -2444,46 +2465,48 @@
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
     </row>
-    <row r="58" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A58" s="33">
+    <row r="58" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A58" s="32">
+        <v>1</v>
+      </c>
+      <c r="B58" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="C58" s="83"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+    </row>
+    <row r="59" spans="1:17" ht="26" x14ac:dyDescent="0.25">
+      <c r="A59" s="33">
         <v>2</v>
       </c>
-      <c r="B58" s="34" t="s">
+      <c r="B59" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="34"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="20"/>
-      <c r="J58" s="20"/>
-      <c r="K58" s="18"/>
-    </row>
-    <row r="59" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A59" s="33">
+      <c r="C59" s="34"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="18"/>
+    </row>
+    <row r="60" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A60" s="33">
         <v>3</v>
       </c>
-      <c r="B59" s="34" t="s">
+      <c r="B60" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C59" s="34"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="18"/>
-    </row>
-    <row r="60" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A60" s="104" t="s">
-        <v>23</v>
-      </c>
-      <c r="B60" s="104"/>
-      <c r="C60" s="104"/>
+      <c r="C60" s="34"/>
       <c r="D60" s="18"/>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
@@ -2493,38 +2516,38 @@
       <c r="J60" s="18"/>
       <c r="K60" s="18"/>
     </row>
-    <row r="61" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
-      <c r="J61" s="20"/>
+    <row r="61" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+      <c r="A61" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" s="71"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
       <c r="K61" s="18"/>
     </row>
-    <row r="62" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" ht="26" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
-      <c r="J62" s="18"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
       <c r="K62" s="18"/>
     </row>
-    <row r="63" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A63" s="104" t="s">
-        <v>24</v>
-      </c>
-      <c r="B63" s="104"/>
-      <c r="C63" s="104"/>
+    <row r="63" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
@@ -2534,42 +2557,42 @@
       <c r="J63" s="18"/>
       <c r="K63" s="18"/>
     </row>
-    <row r="64" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A64" s="34">
+    <row r="64" spans="1:17" ht="26" x14ac:dyDescent="0.2">
+      <c r="A64" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" s="71"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+    </row>
+    <row r="65" spans="1:11" ht="26" x14ac:dyDescent="0.25">
+      <c r="A65" s="34">
         <v>1</v>
       </c>
-      <c r="B64" s="139" t="s">
+      <c r="B65" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="C64" s="141"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="20"/>
-      <c r="I64" s="20"/>
-      <c r="J64" s="20"/>
-      <c r="K64" s="18"/>
-    </row>
-    <row r="65" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="18"/>
-      <c r="H65" s="18"/>
-      <c r="I65" s="18"/>
-      <c r="J65" s="18"/>
+      <c r="C65" s="84"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="20"/>
       <c r="K65" s="18"/>
     </row>
-    <row r="66" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A66" s="104" t="s">
-        <v>25</v>
-      </c>
-      <c r="B66" s="104"/>
-      <c r="C66" s="104"/>
+    <row r="66" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
       <c r="D66" s="18"/>
       <c r="E66" s="18"/>
       <c r="F66" s="18"/>
@@ -2579,103 +2602,116 @@
       <c r="J66" s="18"/>
       <c r="K66" s="18"/>
     </row>
-    <row r="67" spans="1:11" ht="26" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="20"/>
-      <c r="H67" s="20"/>
-      <c r="I67" s="20"/>
-      <c r="J67" s="20"/>
-    </row>
-    <row r="68" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A67" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67" s="71"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+    </row>
+    <row r="68" spans="1:11" ht="26" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A69" s="104" t="s">
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="20"/>
+      <c r="I68" s="20"/>
+      <c r="J68" s="20"/>
+    </row>
+    <row r="69" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A70" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="B69" s="104"/>
-      <c r="C69" s="104"/>
-    </row>
-    <row r="72" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A72" s="104" t="s">
+      <c r="B70" s="71"/>
+      <c r="C70" s="71"/>
+    </row>
+    <row r="73" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A73" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="B72" s="104"/>
-      <c r="C72" s="105"/>
-    </row>
-    <row r="73" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
+      <c r="B73" s="71"/>
+      <c r="C73" s="72"/>
     </row>
     <row r="74" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
+    <row r="75" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="114">
-    <mergeCell ref="H2:J3"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
+  <mergeCells count="118">
+    <mergeCell ref="H23:P23"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:P17"/>
+    <mergeCell ref="H13:P13"/>
+    <mergeCell ref="H12:P12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H15:P15"/>
+    <mergeCell ref="H19:P19"/>
+    <mergeCell ref="H21:P21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H22:P22"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H18:P18"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="H6:P6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
@@ -2694,48 +2730,54 @@
     <mergeCell ref="H11:P11"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="H9:P9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="H2:J3"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A37:C37"/>
     <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:P17"/>
-    <mergeCell ref="H13:P13"/>
-    <mergeCell ref="H12:P12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H15:P15"/>
-    <mergeCell ref="H19:P19"/>
-    <mergeCell ref="H21:P21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H22:P22"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H18:P18"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="F30:G30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
bs; 2dbs; koko eating bananas reviewed
</commit_message>
<xml_diff>
--- a/neetcode_150/neetcode150_fast_reviews.xlsx
+++ b/neetcode_150/neetcode150_fast_reviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mys1erious/Desktop/StudyProgramming/Git/algorithms/neetcode_150/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D31A8F-8180-9D4C-93AD-B2093CA11A32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5553D8BD-0609-2941-AD2F-2523D98B8401}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="920" windowWidth="28040" windowHeight="17440" xr2:uid="{76CD3ECE-D592-4947-8368-191EE7B52C35}"/>
+    <workbookView xWindow="3560" yWindow="880" windowWidth="28040" windowHeight="17440" xr2:uid="{76CD3ECE-D592-4947-8368-191EE7B52C35}"/>
   </bookViews>
   <sheets>
     <sheet name="Neetcode150" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="112">
   <si>
     <t>Arrays and Hashing</t>
   </si>
@@ -352,13 +352,31 @@
   </si>
   <si>
     <t>sort pos, speed; for each car calculate left distance and left time to get to dest; then if cur car takes longer time to get to dest than the prev one, make prev=cur, increase car fleet</t>
+  </si>
+  <si>
+    <t>T: O(logn)</t>
+  </si>
+  <si>
+    <t>default binary search</t>
+  </si>
+  <si>
+    <t>treat matrix as normal array in bs; rp=m*n-1; get rowp as mp//n, colp as mp%n</t>
+  </si>
+  <si>
+    <t>T: O(log(nm))</t>
+  </si>
+  <si>
+    <t>T: O(log(max(p)n))</t>
+  </si>
+  <si>
+    <t>range of k is 1…max(p); use binary search on that range; check if cur_h &lt; h: make k=min(k, mp), rp=mp-1; if cur_h &gt; h: lp=mp+1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -432,6 +450,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="6">
@@ -595,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -712,7 +740,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -795,22 +822,52 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -819,48 +876,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -870,6 +912,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -879,111 +1020,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -993,7 +1038,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1014,17 +1059,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1049,6 +1097,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1366,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662B42D0-2FDD-8740-B5DE-63A10E0A48C3}">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38:G38"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1380,54 +1431,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="145" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="140"/>
+      <c r="B1" s="145"/>
       <c r="C1" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="141" t="s">
+      <c r="D1" s="146" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="141"/>
-      <c r="F1" s="142" t="s">
+      <c r="E1" s="146"/>
+      <c r="F1" s="147" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="142"/>
+      <c r="G1" s="147"/>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="149" t="s">
+      <c r="C2" s="144"/>
+      <c r="D2" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="135" t="s">
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
     </row>
     <row r="3" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="135"/>
-      <c r="B3" s="135"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149"/>
-      <c r="F3" s="149"/>
-      <c r="G3" s="149"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="154"/>
+      <c r="E3" s="154"/>
+      <c r="F3" s="154"/>
+      <c r="G3" s="154"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
       <c r="K3" s="42"/>
       <c r="L3" s="42"/>
       <c r="M3" s="42"/>
@@ -1436,11 +1487,11 @@
       <c r="P3" s="43"/>
     </row>
     <row r="4" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A4" s="144" t="s">
+      <c r="A4" s="149" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="144"/>
-      <c r="C4" s="144"/>
+      <c r="B4" s="149"/>
+      <c r="C4" s="149"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -1453,18 +1504,18 @@
       <c r="A5" s="8">
         <v>1</v>
       </c>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="138" t="s">
+      <c r="C5" s="91"/>
+      <c r="D5" s="136" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138" t="s">
+      <c r="E5" s="136"/>
+      <c r="F5" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="138"/>
+      <c r="G5" s="136"/>
       <c r="H5" s="4" t="s">
         <v>47</v>
       </c>
@@ -1480,57 +1531,57 @@
       <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="123" t="s">
+      <c r="C6" s="91"/>
+      <c r="D6" s="135" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="121"/>
-      <c r="F6" s="138" t="s">
+      <c r="E6" s="122"/>
+      <c r="F6" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="139"/>
-      <c r="H6" s="136" t="s">
+      <c r="G6" s="137"/>
+      <c r="H6" s="133" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="137"/>
-      <c r="J6" s="137"/>
-      <c r="K6" s="137"/>
-      <c r="L6" s="137"/>
-      <c r="M6" s="137"/>
-      <c r="N6" s="137"/>
-      <c r="O6" s="137"/>
-      <c r="P6" s="137"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="134"/>
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
     </row>
     <row r="7" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>3</v>
       </c>
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="123" t="s">
+      <c r="C7" s="91"/>
+      <c r="D7" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="121"/>
-      <c r="F7" s="138" t="s">
+      <c r="E7" s="122"/>
+      <c r="F7" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="139"/>
-      <c r="H7" s="136" t="s">
+      <c r="G7" s="137"/>
+      <c r="H7" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="137"/>
-      <c r="J7" s="137"/>
-      <c r="K7" s="137"/>
-      <c r="L7" s="137"/>
-      <c r="M7" s="137"/>
-      <c r="N7" s="137"/>
-      <c r="O7" s="137"/>
-      <c r="P7" s="137"/>
+      <c r="I7" s="134"/>
+      <c r="J7" s="134"/>
+      <c r="K7" s="134"/>
+      <c r="L7" s="134"/>
+      <c r="M7" s="134"/>
+      <c r="N7" s="134"/>
+      <c r="O7" s="134"/>
+      <c r="P7" s="134"/>
       <c r="Q7" s="5" t="s">
         <v>35</v>
       </c>
@@ -1539,29 +1590,29 @@
       <c r="A8" s="14">
         <v>4</v>
       </c>
-      <c r="B8" s="154" t="s">
+      <c r="B8" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="155"/>
-      <c r="D8" s="123" t="s">
+      <c r="C8" s="161"/>
+      <c r="D8" s="135" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="121"/>
-      <c r="F8" s="138" t="s">
+      <c r="E8" s="122"/>
+      <c r="F8" s="136" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="139"/>
-      <c r="H8" s="86" t="s">
+      <c r="G8" s="137"/>
+      <c r="H8" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="87"/>
-      <c r="J8" s="87"/>
-      <c r="K8" s="87"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="87"/>
-      <c r="N8" s="87"/>
-      <c r="O8" s="87"/>
-      <c r="P8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="89"/>
     </row>
     <row r="9" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="33">
@@ -1571,53 +1622,53 @@
         <v>56</v>
       </c>
       <c r="C9" s="34"/>
-      <c r="D9" s="123" t="s">
+      <c r="D9" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="121"/>
-      <c r="F9" s="104" t="s">
+      <c r="E9" s="122"/>
+      <c r="F9" s="141" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="85"/>
-      <c r="H9" s="99" t="s">
+      <c r="G9" s="102"/>
+      <c r="H9" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="I9" s="100"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="100"/>
-      <c r="L9" s="100"/>
-      <c r="M9" s="100"/>
-      <c r="N9" s="100"/>
-      <c r="O9" s="100"/>
-      <c r="P9" s="101"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="104"/>
+      <c r="N9" s="104"/>
+      <c r="O9" s="104"/>
+      <c r="P9" s="105"/>
     </row>
     <row r="10" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="33">
         <v>6</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="83" t="s">
+      <c r="C10" s="90"/>
+      <c r="D10" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84" t="s">
+      <c r="E10" s="93"/>
+      <c r="F10" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="85"/>
-      <c r="H10" s="100" t="s">
+      <c r="G10" s="102"/>
+      <c r="H10" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="100"/>
-      <c r="J10" s="100"/>
-      <c r="K10" s="100"/>
-      <c r="L10" s="100"/>
-      <c r="M10" s="100"/>
-      <c r="N10" s="100"/>
-      <c r="O10" s="100"/>
-      <c r="P10" s="101"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="104"/>
+      <c r="N10" s="104"/>
+      <c r="O10" s="104"/>
+      <c r="P10" s="105"/>
     </row>
     <row r="11" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="36">
@@ -1627,744 +1678,763 @@
         <v>60</v>
       </c>
       <c r="C11" s="36"/>
-      <c r="D11" s="124" t="s">
+      <c r="D11" s="138" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102" t="s">
+      <c r="E11" s="139"/>
+      <c r="F11" s="139" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="103"/>
-      <c r="H11" s="100" t="s">
+      <c r="G11" s="140"/>
+      <c r="H11" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="100"/>
-      <c r="J11" s="100"/>
-      <c r="K11" s="100"/>
-      <c r="L11" s="100"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="100"/>
-      <c r="O11" s="100"/>
-      <c r="P11" s="101"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="104"/>
+      <c r="N11" s="104"/>
+      <c r="O11" s="104"/>
+      <c r="P11" s="105"/>
     </row>
     <row r="12" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="41">
         <v>8</v>
       </c>
-      <c r="B12" s="159" t="s">
+      <c r="B12" s="165" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="160"/>
+      <c r="C12" s="166"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="114" t="s">
+      <c r="H12" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="115"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="115"/>
-      <c r="L12" s="115"/>
-      <c r="M12" s="115"/>
-      <c r="N12" s="115"/>
-      <c r="O12" s="115"/>
-      <c r="P12" s="116"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="116"/>
+      <c r="L12" s="116"/>
+      <c r="M12" s="116"/>
+      <c r="N12" s="116"/>
+      <c r="O12" s="116"/>
+      <c r="P12" s="117"/>
     </row>
     <row r="13" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="47">
+      <c r="A13" s="46">
         <v>9</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="117" t="s">
+      <c r="C13" s="47"/>
+      <c r="D13" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118" t="s">
+      <c r="E13" s="119"/>
+      <c r="F13" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="119"/>
-      <c r="H13" s="111" t="s">
+      <c r="G13" s="120"/>
+      <c r="H13" s="112" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="112"/>
-      <c r="J13" s="112"/>
-      <c r="K13" s="112"/>
-      <c r="L13" s="112"/>
-      <c r="M13" s="112"/>
-      <c r="N13" s="112"/>
-      <c r="O13" s="112"/>
-      <c r="P13" s="113"/>
+      <c r="I13" s="113"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="113"/>
+      <c r="L13" s="113"/>
+      <c r="M13" s="113"/>
+      <c r="N13" s="113"/>
+      <c r="O13" s="113"/>
+      <c r="P13" s="114"/>
     </row>
     <row r="14" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="144"/>
-      <c r="C14" s="145"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="66"/>
-      <c r="N14" s="66"/>
-      <c r="O14" s="66"/>
-      <c r="P14" s="67"/>
+      <c r="B14" s="149"/>
+      <c r="C14" s="150"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="66"/>
       <c r="Q14" s="17"/>
     </row>
     <row r="15" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52">
+      <c r="A15" s="51">
         <v>1</v>
       </c>
-      <c r="B15" s="129" t="s">
+      <c r="B15" s="127" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="130"/>
-      <c r="D15" s="109" t="s">
+      <c r="C15" s="128"/>
+      <c r="D15" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109" t="s">
+      <c r="E15" s="110"/>
+      <c r="F15" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="109"/>
-      <c r="H15" s="86" t="s">
+      <c r="G15" s="110"/>
+      <c r="H15" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="I15" s="87"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="87"/>
-      <c r="L15" s="87"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="87"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="88"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="88"/>
+      <c r="O15" s="88"/>
+      <c r="P15" s="89"/>
       <c r="Q15" s="17"/>
     </row>
     <row r="16" spans="1:17" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="54">
+      <c r="A16" s="53">
         <v>2</v>
       </c>
-      <c r="B16" s="129" t="s">
+      <c r="B16" s="127" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="130"/>
-      <c r="D16" s="108" t="s">
+      <c r="C16" s="128"/>
+      <c r="D16" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109" t="s">
+      <c r="E16" s="110"/>
+      <c r="F16" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="110"/>
-      <c r="H16" s="86" t="s">
+      <c r="G16" s="111"/>
+      <c r="H16" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="87"/>
-      <c r="J16" s="87"/>
-      <c r="K16" s="87"/>
-      <c r="L16" s="87"/>
-      <c r="M16" s="87"/>
-      <c r="N16" s="87"/>
-      <c r="O16" s="87"/>
-      <c r="P16" s="88"/>
+      <c r="I16" s="88"/>
+      <c r="J16" s="88"/>
+      <c r="K16" s="88"/>
+      <c r="L16" s="88"/>
+      <c r="M16" s="88"/>
+      <c r="N16" s="88"/>
+      <c r="O16" s="88"/>
+      <c r="P16" s="89"/>
       <c r="Q16" s="17"/>
     </row>
     <row r="17" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="54">
+      <c r="A17" s="53">
         <v>3</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="108" t="s">
+      <c r="C17" s="49"/>
+      <c r="D17" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109" t="s">
+      <c r="E17" s="110"/>
+      <c r="F17" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="110"/>
-      <c r="H17" s="86" t="s">
+      <c r="G17" s="111"/>
+      <c r="H17" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="I17" s="87"/>
-      <c r="J17" s="87"/>
-      <c r="K17" s="87"/>
-      <c r="L17" s="87"/>
-      <c r="M17" s="87"/>
-      <c r="N17" s="87"/>
-      <c r="O17" s="87"/>
-      <c r="P17" s="88"/>
+      <c r="I17" s="88"/>
+      <c r="J17" s="88"/>
+      <c r="K17" s="88"/>
+      <c r="L17" s="88"/>
+      <c r="M17" s="88"/>
+      <c r="N17" s="88"/>
+      <c r="O17" s="88"/>
+      <c r="P17" s="89"/>
       <c r="Q17" s="17"/>
     </row>
     <row r="18" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="54">
+      <c r="A18" s="53">
         <v>4</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="108" t="s">
+      <c r="C18" s="49"/>
+      <c r="D18" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109" t="s">
+      <c r="E18" s="110"/>
+      <c r="F18" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="110"/>
-      <c r="H18" s="86" t="s">
+      <c r="G18" s="111"/>
+      <c r="H18" s="87" t="s">
         <v>78</v>
       </c>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="87"/>
-      <c r="P18" s="88"/>
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="88"/>
+      <c r="L18" s="88"/>
+      <c r="M18" s="88"/>
+      <c r="N18" s="88"/>
+      <c r="O18" s="88"/>
+      <c r="P18" s="89"/>
       <c r="Q18" s="17"/>
     </row>
     <row r="19" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="53">
+      <c r="A19" s="52">
         <v>5</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="91" t="s">
+      <c r="C19" s="55"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="92"/>
-      <c r="J19" s="92"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="92"/>
-      <c r="M19" s="92"/>
-      <c r="N19" s="92"/>
-      <c r="O19" s="92"/>
-      <c r="P19" s="93"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="97"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="97"/>
+      <c r="M19" s="97"/>
+      <c r="N19" s="97"/>
+      <c r="O19" s="97"/>
+      <c r="P19" s="98"/>
       <c r="Q19" s="17"/>
     </row>
     <row r="20" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="144" t="s">
+      <c r="A20" s="149" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="144"/>
-      <c r="C20" s="145"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="72"/>
-      <c r="O20" s="72"/>
-      <c r="P20" s="73"/>
+      <c r="B20" s="149"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="71"/>
+      <c r="P20" s="72"/>
       <c r="Q20" s="17"/>
     </row>
     <row r="21" spans="1:17" ht="19" x14ac:dyDescent="0.2">
-      <c r="A21" s="57">
+      <c r="A21" s="56">
         <v>1</v>
       </c>
-      <c r="B21" s="129" t="s">
+      <c r="B21" s="127" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="130"/>
-      <c r="D21" s="83" t="s">
+      <c r="C21" s="128"/>
+      <c r="D21" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="84"/>
-      <c r="F21" s="84" t="s">
+      <c r="E21" s="93"/>
+      <c r="F21" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="85"/>
-      <c r="H21" s="99" t="s">
+      <c r="G21" s="102"/>
+      <c r="H21" s="103" t="s">
         <v>83</v>
       </c>
-      <c r="I21" s="100"/>
-      <c r="J21" s="100"/>
-      <c r="K21" s="100"/>
-      <c r="L21" s="100"/>
-      <c r="M21" s="100"/>
-      <c r="N21" s="100"/>
-      <c r="O21" s="100"/>
-      <c r="P21" s="101"/>
+      <c r="I21" s="104"/>
+      <c r="J21" s="104"/>
+      <c r="K21" s="104"/>
+      <c r="L21" s="104"/>
+      <c r="M21" s="104"/>
+      <c r="N21" s="104"/>
+      <c r="O21" s="104"/>
+      <c r="P21" s="105"/>
       <c r="Q21" s="17"/>
     </row>
     <row r="22" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="59">
+      <c r="A22" s="58">
         <v>2</v>
       </c>
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="83" t="s">
+      <c r="C22" s="57"/>
+      <c r="D22" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="84"/>
-      <c r="F22" s="84" t="s">
+      <c r="E22" s="93"/>
+      <c r="F22" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="85"/>
-      <c r="H22" s="99" t="s">
+      <c r="G22" s="102"/>
+      <c r="H22" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="I22" s="100"/>
-      <c r="J22" s="100"/>
-      <c r="K22" s="100"/>
-      <c r="L22" s="100"/>
-      <c r="M22" s="100"/>
-      <c r="N22" s="100"/>
-      <c r="O22" s="100"/>
-      <c r="P22" s="101"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="104"/>
+      <c r="O22" s="104"/>
+      <c r="P22" s="105"/>
       <c r="Q22" s="17"/>
     </row>
     <row r="23" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="62">
+      <c r="A23" s="61">
         <v>3</v>
       </c>
-      <c r="B23" s="97" t="s">
+      <c r="B23" s="90" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="98"/>
-      <c r="D23" s="83" t="s">
+      <c r="C23" s="91"/>
+      <c r="D23" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84" t="s">
+      <c r="E23" s="93"/>
+      <c r="F23" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="85"/>
-      <c r="H23" s="99" t="s">
+      <c r="G23" s="102"/>
+      <c r="H23" s="103" t="s">
         <v>87</v>
       </c>
-      <c r="I23" s="100"/>
-      <c r="J23" s="100"/>
-      <c r="K23" s="100"/>
-      <c r="L23" s="100"/>
-      <c r="M23" s="100"/>
-      <c r="N23" s="100"/>
-      <c r="O23" s="100"/>
-      <c r="P23" s="101"/>
+      <c r="I23" s="104"/>
+      <c r="J23" s="104"/>
+      <c r="K23" s="104"/>
+      <c r="L23" s="104"/>
+      <c r="M23" s="104"/>
+      <c r="N23" s="104"/>
+      <c r="O23" s="104"/>
+      <c r="P23" s="105"/>
       <c r="Q23" s="17"/>
     </row>
     <row r="24" spans="1:17" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="62">
+      <c r="A24" s="61">
         <v>4</v>
       </c>
-      <c r="B24" s="97" t="s">
+      <c r="B24" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="98"/>
-      <c r="D24" s="83" t="s">
+      <c r="C24" s="91"/>
+      <c r="D24" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84" t="s">
+      <c r="E24" s="93"/>
+      <c r="F24" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="85"/>
-      <c r="H24" s="99" t="s">
+      <c r="G24" s="102"/>
+      <c r="H24" s="103" t="s">
         <v>89</v>
       </c>
-      <c r="I24" s="100"/>
-      <c r="J24" s="100"/>
-      <c r="K24" s="100"/>
-      <c r="L24" s="100"/>
-      <c r="M24" s="100"/>
-      <c r="N24" s="100"/>
-      <c r="O24" s="100"/>
-      <c r="P24" s="101"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="104"/>
+      <c r="M24" s="104"/>
+      <c r="N24" s="104"/>
+      <c r="O24" s="104"/>
+      <c r="P24" s="105"/>
       <c r="Q24" s="17"/>
     </row>
     <row r="25" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="63">
+      <c r="A25" s="62">
         <v>5</v>
       </c>
-      <c r="B25" s="81" t="s">
+      <c r="B25" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="82"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="91" t="s">
+      <c r="C25" s="95"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="I25" s="92"/>
-      <c r="J25" s="92"/>
-      <c r="K25" s="92"/>
-      <c r="L25" s="92"/>
-      <c r="M25" s="92"/>
-      <c r="N25" s="92"/>
-      <c r="O25" s="92"/>
-      <c r="P25" s="93"/>
+      <c r="I25" s="97"/>
+      <c r="J25" s="97"/>
+      <c r="K25" s="97"/>
+      <c r="L25" s="97"/>
+      <c r="M25" s="97"/>
+      <c r="N25" s="97"/>
+      <c r="O25" s="97"/>
+      <c r="P25" s="98"/>
       <c r="Q25" s="17"/>
     </row>
     <row r="26" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="61">
+      <c r="A26" s="60">
         <v>6</v>
       </c>
-      <c r="B26" s="81" t="s">
+      <c r="B26" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="82"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="91" t="s">
+      <c r="C26" s="95"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="I26" s="92"/>
-      <c r="J26" s="92"/>
-      <c r="K26" s="92"/>
-      <c r="L26" s="92"/>
-      <c r="M26" s="92"/>
-      <c r="N26" s="92"/>
-      <c r="O26" s="92"/>
-      <c r="P26" s="93"/>
+      <c r="I26" s="97"/>
+      <c r="J26" s="97"/>
+      <c r="K26" s="97"/>
+      <c r="L26" s="97"/>
+      <c r="M26" s="97"/>
+      <c r="N26" s="97"/>
+      <c r="O26" s="97"/>
+      <c r="P26" s="98"/>
       <c r="Q26" s="17"/>
     </row>
     <row r="27" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="146" t="s">
+      <c r="A27" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="146"/>
-      <c r="C27" s="146"/>
-      <c r="D27" s="152"/>
-      <c r="E27" s="153"/>
-      <c r="F27" s="153"/>
-      <c r="G27" s="153"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="66"/>
-      <c r="L27" s="66"/>
-      <c r="M27" s="66"/>
-      <c r="N27" s="66"/>
-      <c r="O27" s="66"/>
-      <c r="P27" s="67"/>
+      <c r="B27" s="151"/>
+      <c r="C27" s="151"/>
+      <c r="D27" s="142"/>
+      <c r="E27" s="143"/>
+      <c r="F27" s="143"/>
+      <c r="G27" s="143"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="66"/>
       <c r="Q27" s="17"/>
     </row>
     <row r="28" spans="1:17" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="76">
+      <c r="A28" s="75">
         <v>1</v>
       </c>
-      <c r="B28" s="147" t="s">
+      <c r="B28" s="152" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="148"/>
-      <c r="D28" s="121" t="s">
+      <c r="C28" s="153"/>
+      <c r="D28" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="121"/>
-      <c r="F28" s="121" t="s">
+      <c r="E28" s="122"/>
+      <c r="F28" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="121"/>
-      <c r="H28" s="94" t="s">
+      <c r="G28" s="122"/>
+      <c r="H28" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="I28" s="95"/>
-      <c r="J28" s="95"/>
-      <c r="K28" s="95"/>
-      <c r="L28" s="95"/>
-      <c r="M28" s="95"/>
-      <c r="N28" s="95"/>
-      <c r="O28" s="95"/>
-      <c r="P28" s="96"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="100"/>
+      <c r="K28" s="100"/>
+      <c r="L28" s="100"/>
+      <c r="M28" s="100"/>
+      <c r="N28" s="100"/>
+      <c r="O28" s="100"/>
+      <c r="P28" s="101"/>
       <c r="Q28" s="17"/>
     </row>
     <row r="29" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>2</v>
       </c>
-      <c r="B29" s="97" t="s">
+      <c r="B29" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="98"/>
-      <c r="D29" s="84" t="s">
+      <c r="C29" s="91"/>
+      <c r="D29" s="93" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="84"/>
-      <c r="F29" s="84" t="s">
+      <c r="E29" s="93"/>
+      <c r="F29" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="84"/>
-      <c r="H29" s="86" t="s">
+      <c r="G29" s="93"/>
+      <c r="H29" s="87" t="s">
         <v>94</v>
       </c>
-      <c r="I29" s="87"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="87"/>
-      <c r="O29" s="87"/>
-      <c r="P29" s="88"/>
+      <c r="I29" s="88"/>
+      <c r="J29" s="88"/>
+      <c r="K29" s="88"/>
+      <c r="L29" s="88"/>
+      <c r="M29" s="88"/>
+      <c r="N29" s="88"/>
+      <c r="O29" s="88"/>
+      <c r="P29" s="89"/>
       <c r="Q29" s="17"/>
     </row>
     <row r="30" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="74">
+      <c r="A30" s="73">
         <v>3</v>
       </c>
-      <c r="B30" s="97" t="s">
+      <c r="B30" s="90" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="98"/>
-      <c r="D30" s="83" t="s">
+      <c r="C30" s="91"/>
+      <c r="D30" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="84"/>
-      <c r="F30" s="84" t="s">
+      <c r="E30" s="93"/>
+      <c r="F30" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="85"/>
-      <c r="H30" s="86" t="s">
+      <c r="G30" s="102"/>
+      <c r="H30" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="I30" s="87"/>
-      <c r="J30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="M30" s="87"/>
-      <c r="N30" s="87"/>
-      <c r="O30" s="87"/>
-      <c r="P30" s="88"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="88"/>
+      <c r="M30" s="88"/>
+      <c r="N30" s="88"/>
+      <c r="O30" s="88"/>
+      <c r="P30" s="89"/>
       <c r="Q30" s="17"/>
     </row>
     <row r="31" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="78">
+      <c r="A31" s="76">
         <v>4</v>
       </c>
-      <c r="B31" s="97" t="s">
+      <c r="B31" s="90" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="98"/>
-      <c r="D31" s="83" t="s">
+      <c r="C31" s="91"/>
+      <c r="D31" s="92" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="84"/>
-      <c r="F31" s="84" t="s">
+      <c r="E31" s="93"/>
+      <c r="F31" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="85"/>
-      <c r="H31" s="86" t="s">
+      <c r="G31" s="102"/>
+      <c r="H31" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="I31" s="87"/>
-      <c r="J31" s="87"/>
-      <c r="K31" s="87"/>
-      <c r="L31" s="87"/>
-      <c r="M31" s="87"/>
-      <c r="N31" s="87"/>
-      <c r="O31" s="87"/>
-      <c r="P31" s="88"/>
+      <c r="I31" s="88"/>
+      <c r="J31" s="88"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="88"/>
+      <c r="M31" s="88"/>
+      <c r="N31" s="88"/>
+      <c r="O31" s="88"/>
+      <c r="P31" s="89"/>
       <c r="Q31" s="17"/>
     </row>
     <row r="32" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="77">
         <v>5</v>
       </c>
-      <c r="B32" s="89" t="s">
+      <c r="B32" s="90" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="90"/>
-      <c r="D32" s="83" t="s">
+      <c r="C32" s="91"/>
+      <c r="D32" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84" t="s">
+      <c r="E32" s="93"/>
+      <c r="F32" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="85"/>
-      <c r="H32" s="86" t="s">
+      <c r="G32" s="102"/>
+      <c r="H32" s="87" t="s">
         <v>100</v>
       </c>
-      <c r="I32" s="87"/>
-      <c r="J32" s="87"/>
-      <c r="K32" s="87"/>
-      <c r="L32" s="87"/>
-      <c r="M32" s="87"/>
-      <c r="N32" s="87"/>
-      <c r="O32" s="87"/>
-      <c r="P32" s="88"/>
+      <c r="I32" s="88"/>
+      <c r="J32" s="88"/>
+      <c r="K32" s="88"/>
+      <c r="L32" s="88"/>
+      <c r="M32" s="88"/>
+      <c r="N32" s="88"/>
+      <c r="O32" s="88"/>
+      <c r="P32" s="89"/>
       <c r="Q32" s="17"/>
     </row>
     <row r="33" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="80">
+      <c r="A33" s="77">
         <v>6</v>
       </c>
-      <c r="B33" s="89" t="s">
+      <c r="B33" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="90"/>
-      <c r="D33" s="83" t="s">
+      <c r="C33" s="91"/>
+      <c r="D33" s="92" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84" t="s">
+      <c r="E33" s="93"/>
+      <c r="F33" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="85"/>
-      <c r="H33" s="86" t="s">
+      <c r="G33" s="102"/>
+      <c r="H33" s="87" t="s">
         <v>105</v>
       </c>
-      <c r="I33" s="87"/>
-      <c r="J33" s="87"/>
-      <c r="K33" s="87"/>
-      <c r="L33" s="87"/>
-      <c r="M33" s="87"/>
-      <c r="N33" s="87"/>
-      <c r="O33" s="87"/>
-      <c r="P33" s="88"/>
+      <c r="I33" s="88"/>
+      <c r="J33" s="88"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="88"/>
+      <c r="M33" s="88"/>
+      <c r="N33" s="88"/>
+      <c r="O33" s="88"/>
+      <c r="P33" s="89"/>
       <c r="Q33" s="17"/>
     </row>
     <row r="34" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="79">
+      <c r="A34" s="54">
         <v>7</v>
       </c>
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="158" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="82"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="84"/>
-      <c r="F34" s="84"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="91" t="s">
+      <c r="C34" s="159"/>
+      <c r="D34" s="92"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="102"/>
+      <c r="H34" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="I34" s="92"/>
-      <c r="J34" s="92"/>
-      <c r="K34" s="92"/>
-      <c r="L34" s="92"/>
-      <c r="M34" s="92"/>
-      <c r="N34" s="92"/>
-      <c r="O34" s="92"/>
-      <c r="P34" s="93"/>
+      <c r="I34" s="97"/>
+      <c r="J34" s="97"/>
+      <c r="K34" s="97"/>
+      <c r="L34" s="97"/>
+      <c r="M34" s="97"/>
+      <c r="N34" s="97"/>
+      <c r="O34" s="97"/>
+      <c r="P34" s="98"/>
       <c r="Q34" s="17"/>
     </row>
     <row r="35" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="150" t="s">
+      <c r="A35" s="155" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="150"/>
-      <c r="C35" s="151"/>
-      <c r="D35" s="143"/>
-      <c r="E35" s="143"/>
-      <c r="F35" s="143"/>
-      <c r="G35" s="143"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="37"/>
-      <c r="P35" s="45"/>
+      <c r="B35" s="156"/>
+      <c r="C35" s="157"/>
+      <c r="D35" s="148"/>
+      <c r="E35" s="148"/>
+      <c r="F35" s="148"/>
+      <c r="G35" s="148"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="71"/>
+      <c r="M35" s="71"/>
+      <c r="N35" s="71"/>
+      <c r="O35" s="71"/>
+      <c r="P35" s="72"/>
       <c r="Q35" s="17"/>
     </row>
     <row r="36" spans="1:17" ht="26" x14ac:dyDescent="0.2">
-      <c r="A36" s="24">
+      <c r="A36" s="78">
         <v>1</v>
       </c>
-      <c r="B36" s="131" t="s">
+      <c r="B36" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="132"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="17"/>
-      <c r="P36" s="46"/>
+      <c r="C36" s="128"/>
+      <c r="D36" s="109" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="110"/>
+      <c r="F36" s="82" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="83"/>
+      <c r="H36" s="79" t="s">
+        <v>107</v>
+      </c>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="80"/>
+      <c r="M36" s="80"/>
+      <c r="N36" s="80"/>
+      <c r="O36" s="80"/>
+      <c r="P36" s="81"/>
       <c r="Q36" s="17"/>
     </row>
-    <row r="37" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="24">
+    <row r="37" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="8">
         <v>2</v>
       </c>
-      <c r="B37" s="131" t="s">
+      <c r="B37" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="132"/>
-      <c r="D37" s="107"/>
-      <c r="E37" s="107"/>
-      <c r="F37" s="107"/>
-      <c r="G37" s="107"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="46"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="108" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="108"/>
+      <c r="F37" s="108" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="108"/>
+      <c r="H37" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="I37" s="85"/>
+      <c r="J37" s="85"/>
+      <c r="K37" s="85"/>
+      <c r="L37" s="85"/>
+      <c r="M37" s="85"/>
+      <c r="N37" s="85"/>
+      <c r="O37" s="85"/>
+      <c r="P37" s="86"/>
       <c r="Q37" s="17"/>
     </row>
     <row r="38" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="24">
         <v>3</v>
       </c>
-      <c r="B38" s="131" t="s">
+      <c r="B38" s="129" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="132"/>
-      <c r="D38" s="107"/>
-      <c r="E38" s="107"/>
-      <c r="F38" s="107"/>
-      <c r="G38" s="107"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="37"/>
-      <c r="N38" s="37"/>
-      <c r="O38" s="37"/>
-      <c r="P38" s="45"/>
+      <c r="C38" s="130"/>
+      <c r="D38" s="108" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" s="108"/>
+      <c r="F38" s="108" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="108"/>
+      <c r="H38" s="133" t="s">
+        <v>111</v>
+      </c>
+      <c r="I38" s="134"/>
+      <c r="J38" s="134"/>
+      <c r="K38" s="134"/>
+      <c r="L38" s="134"/>
+      <c r="M38" s="134"/>
+      <c r="N38" s="134"/>
+      <c r="O38" s="134"/>
+      <c r="P38" s="168"/>
       <c r="Q38" s="17"/>
     </row>
     <row r="39" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="23">
         <v>4</v>
       </c>
-      <c r="B39" s="131" t="s">
+      <c r="B39" s="129" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="132"/>
+      <c r="C39" s="130"/>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
       <c r="F39" s="20"/>
@@ -2381,11 +2451,11 @@
       <c r="Q39" s="17"/>
     </row>
     <row r="40" spans="1:17" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="127" t="s">
+      <c r="A40" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="127"/>
-      <c r="C40" s="128"/>
+      <c r="B40" s="126"/>
+      <c r="C40" s="83"/>
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
@@ -2405,10 +2475,10 @@
       <c r="A41" s="25">
         <v>1</v>
       </c>
-      <c r="B41" s="161" t="s">
+      <c r="B41" s="167" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="161"/>
+      <c r="C41" s="167"/>
       <c r="D41" s="20"/>
       <c r="E41" s="20"/>
       <c r="F41" s="20"/>
@@ -2428,14 +2498,14 @@
       <c r="A42" s="26">
         <v>2</v>
       </c>
-      <c r="B42" s="133" t="s">
+      <c r="B42" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="133"/>
-      <c r="D42" s="107"/>
-      <c r="E42" s="107"/>
-      <c r="F42" s="107"/>
-      <c r="G42" s="107"/>
+      <c r="C42" s="131"/>
+      <c r="D42" s="108"/>
+      <c r="E42" s="108"/>
+      <c r="F42" s="108"/>
+      <c r="G42" s="108"/>
       <c r="H42" s="39"/>
       <c r="I42" s="39"/>
       <c r="J42" s="39"/>
@@ -2451,14 +2521,14 @@
       <c r="A43" s="27">
         <v>3</v>
       </c>
-      <c r="B43" s="131" t="s">
+      <c r="B43" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="131"/>
-      <c r="D43" s="107"/>
-      <c r="E43" s="107"/>
-      <c r="F43" s="107"/>
-      <c r="G43" s="107"/>
+      <c r="C43" s="129"/>
+      <c r="D43" s="108"/>
+      <c r="E43" s="108"/>
+      <c r="F43" s="108"/>
+      <c r="G43" s="108"/>
       <c r="H43" s="38"/>
       <c r="I43" s="40"/>
       <c r="J43" s="40"/>
@@ -2474,10 +2544,10 @@
       <c r="A44" s="28">
         <v>4</v>
       </c>
-      <c r="B44" s="134" t="s">
+      <c r="B44" s="132" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="134"/>
+      <c r="C44" s="132"/>
       <c r="D44" s="35"/>
       <c r="E44" s="35"/>
       <c r="F44" s="35"/>
@@ -2494,11 +2564,11 @@
       <c r="Q44" s="17"/>
     </row>
     <row r="45" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="127" t="s">
+      <c r="A45" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="127"/>
-      <c r="C45" s="127"/>
+      <c r="B45" s="126"/>
+      <c r="C45" s="126"/>
       <c r="D45" s="35"/>
       <c r="E45" s="35"/>
       <c r="F45" s="35"/>
@@ -2518,10 +2588,10 @@
       <c r="A46" s="28">
         <v>1</v>
       </c>
-      <c r="B46" s="134" t="s">
+      <c r="B46" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="134"/>
+      <c r="C46" s="132"/>
       <c r="D46" s="20"/>
       <c r="E46" s="20"/>
       <c r="F46" s="20"/>
@@ -2541,10 +2611,10 @@
       <c r="A47" s="27">
         <v>2</v>
       </c>
-      <c r="B47" s="134" t="s">
+      <c r="B47" s="132" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="134"/>
+      <c r="C47" s="132"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
       <c r="F47" s="20"/>
@@ -2564,10 +2634,10 @@
       <c r="A48" s="29">
         <v>3</v>
       </c>
-      <c r="B48" s="131" t="s">
+      <c r="B48" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="132"/>
+      <c r="C48" s="130"/>
       <c r="D48" s="18"/>
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
@@ -2580,10 +2650,10 @@
       <c r="A49" s="16">
         <v>4</v>
       </c>
-      <c r="B49" s="81" t="s">
+      <c r="B49" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="82"/>
+      <c r="C49" s="95"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
@@ -2593,11 +2663,11 @@
       <c r="J49" s="17"/>
     </row>
     <row r="50" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A50" s="127" t="s">
+      <c r="A50" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="127"/>
-      <c r="C50" s="128"/>
+      <c r="B50" s="126"/>
+      <c r="C50" s="83"/>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
@@ -2631,11 +2701,11 @@
       <c r="J52" s="17"/>
     </row>
     <row r="53" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A53" s="127" t="s">
+      <c r="A53" s="126" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="127"/>
-      <c r="C53" s="127"/>
+      <c r="B53" s="126"/>
+      <c r="C53" s="126"/>
       <c r="D53" s="20"/>
       <c r="E53" s="20"/>
       <c r="F53" s="20"/>
@@ -2669,11 +2739,11 @@
       <c r="J55" s="17"/>
     </row>
     <row r="56" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A56" s="127" t="s">
+      <c r="A56" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="B56" s="127"/>
-      <c r="C56" s="127"/>
+      <c r="B56" s="126"/>
+      <c r="C56" s="126"/>
       <c r="D56" s="20"/>
       <c r="E56" s="20"/>
       <c r="F56" s="20"/>
@@ -2707,11 +2777,11 @@
       <c r="J58" s="17"/>
     </row>
     <row r="59" spans="1:17" ht="26" x14ac:dyDescent="0.25">
-      <c r="A59" s="127" t="s">
+      <c r="A59" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="B59" s="127"/>
-      <c r="C59" s="127"/>
+      <c r="B59" s="126"/>
+      <c r="C59" s="126"/>
       <c r="D59" s="20"/>
       <c r="E59" s="20"/>
       <c r="F59" s="20"/>
@@ -2724,10 +2794,10 @@
       <c r="A60" s="11">
         <v>1</v>
       </c>
-      <c r="B60" s="125" t="s">
+      <c r="B60" s="124" t="s">
         <v>33</v>
       </c>
-      <c r="C60" s="126"/>
+      <c r="C60" s="125"/>
       <c r="D60" s="19"/>
       <c r="E60" s="19"/>
       <c r="F60" s="19"/>
@@ -2740,23 +2810,23 @@
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
-      <c r="D61" s="120"/>
-      <c r="E61" s="105"/>
-      <c r="F61" s="122"/>
-      <c r="G61" s="106"/>
+      <c r="D61" s="121"/>
+      <c r="E61" s="106"/>
+      <c r="F61" s="123"/>
+      <c r="G61" s="107"/>
       <c r="H61" s="13"/>
       <c r="Q61" s="13"/>
     </row>
     <row r="62" spans="1:17" s="12" customFormat="1" ht="26" x14ac:dyDescent="0.25">
-      <c r="A62" s="127" t="s">
+      <c r="A62" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="B62" s="127"/>
-      <c r="C62" s="127"/>
-      <c r="D62" s="120"/>
-      <c r="E62" s="105"/>
-      <c r="F62" s="105"/>
-      <c r="G62" s="106"/>
+      <c r="B62" s="126"/>
+      <c r="C62" s="126"/>
+      <c r="D62" s="121"/>
+      <c r="E62" s="106"/>
+      <c r="F62" s="106"/>
+      <c r="G62" s="107"/>
       <c r="H62" s="13"/>
       <c r="Q62" s="13"/>
     </row>
@@ -2788,11 +2858,11 @@
       <c r="K64" s="17"/>
     </row>
     <row r="65" spans="1:11" ht="26" x14ac:dyDescent="0.25">
-      <c r="A65" s="127" t="s">
+      <c r="A65" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="B65" s="127"/>
-      <c r="C65" s="128"/>
+      <c r="B65" s="126"/>
+      <c r="C65" s="83"/>
       <c r="D65" s="20"/>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
@@ -2806,10 +2876,10 @@
       <c r="A66" s="29">
         <v>1</v>
       </c>
-      <c r="B66" s="156" t="s">
+      <c r="B66" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C66" s="157"/>
+      <c r="C66" s="163"/>
       <c r="D66" s="20"/>
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
@@ -2854,11 +2924,11 @@
       <c r="K68" s="17"/>
     </row>
     <row r="69" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A69" s="127" t="s">
+      <c r="A69" s="126" t="s">
         <v>23</v>
       </c>
-      <c r="B69" s="127"/>
-      <c r="C69" s="127"/>
+      <c r="B69" s="126"/>
+      <c r="C69" s="126"/>
       <c r="D69" s="17"/>
       <c r="E69" s="17"/>
       <c r="F69" s="17"/>
@@ -2895,11 +2965,11 @@
       <c r="K71" s="17"/>
     </row>
     <row r="72" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A72" s="127" t="s">
+      <c r="A72" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="B72" s="127"/>
-      <c r="C72" s="127"/>
+      <c r="B72" s="126"/>
+      <c r="C72" s="126"/>
       <c r="D72" s="17"/>
       <c r="E72" s="17"/>
       <c r="F72" s="17"/>
@@ -2913,10 +2983,10 @@
       <c r="A73" s="31">
         <v>1</v>
       </c>
-      <c r="B73" s="156" t="s">
+      <c r="B73" s="162" t="s">
         <v>32</v>
       </c>
-      <c r="C73" s="158"/>
+      <c r="C73" s="164"/>
       <c r="D73" s="19"/>
       <c r="E73" s="19"/>
       <c r="F73" s="19"/>
@@ -2940,11 +3010,11 @@
       <c r="K74" s="17"/>
     </row>
     <row r="75" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A75" s="127" t="s">
+      <c r="A75" s="126" t="s">
         <v>25</v>
       </c>
-      <c r="B75" s="127"/>
-      <c r="C75" s="127"/>
+      <c r="B75" s="126"/>
+      <c r="C75" s="126"/>
       <c r="D75" s="17"/>
       <c r="E75" s="17"/>
       <c r="F75" s="17"/>
@@ -2972,18 +3042,18 @@
       <c r="C77" s="1"/>
     </row>
     <row r="78" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A78" s="127" t="s">
+      <c r="A78" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="B78" s="127"/>
-      <c r="C78" s="127"/>
+      <c r="B78" s="126"/>
+      <c r="C78" s="126"/>
     </row>
     <row r="81" spans="1:3" ht="26" x14ac:dyDescent="0.2">
-      <c r="A81" s="127" t="s">
+      <c r="A81" s="126" t="s">
         <v>27</v>
       </c>
-      <c r="B81" s="127"/>
-      <c r="C81" s="128"/>
+      <c r="B81" s="126"/>
+      <c r="C81" s="83"/>
     </row>
     <row r="82" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
@@ -2996,11 +3066,7 @@
       <c r="C83" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="148">
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H33:P33"/>
+  <mergeCells count="153">
     <mergeCell ref="H34:P34"/>
     <mergeCell ref="H2:J3"/>
     <mergeCell ref="A81:C81"/>
@@ -3021,11 +3087,7 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="A72:C72"/>
     <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="H30:P30"/>
-    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="H38:P38"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -3045,6 +3107,9 @@
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A35:C35"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="D27:E27"/>
@@ -3056,6 +3121,10 @@
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="B37:C37"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="H6:P6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
@@ -3077,6 +3146,8 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F9:G9"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="A65:C65"/>
     <mergeCell ref="A69:C69"/>
@@ -3098,9 +3169,9 @@
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H23:P23"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="F62:G62"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D17:E17"/>
@@ -3122,10 +3193,12 @@
     <mergeCell ref="F43:G43"/>
     <mergeCell ref="F42:G42"/>
     <mergeCell ref="F61:G61"/>
-    <mergeCell ref="B33:C33"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H30:P30"/>
+    <mergeCell ref="H36:P36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H37:P37"/>
     <mergeCell ref="H31:P31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="H18:P18"/>
@@ -3145,6 +3218,8 @@
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="H32:P32"/>
+    <mergeCell ref="H23:P23"/>
+    <mergeCell ref="H33:P33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
max depth of bt, palindrome
</commit_message>
<xml_diff>
--- a/neetcode_150/neetcode150_fast_reviews.xlsx
+++ b/neetcode_150/neetcode150_fast_reviews.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="123">
   <si>
     <t xml:space="preserve">Only revise</t>
   </si>
@@ -307,7 +307,19 @@
     <t xml:space="preserve">Reverse Linked List</t>
   </si>
   <si>
+    <t xml:space="preserve">maintain next variable as cur.next; assing cur.next to prev; move prev, cur pointers to its next val</t>
+  </si>
+  <si>
     <t xml:space="preserve">Merge 2 linked lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T: O(min(m, n))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M: P(m+n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">init merged with dummy node and init a tail for merged; while list1 and list2, add lowest val to merged from cur list1, list2 values; then if list1 or list2 is still not empty, add it to the end of the tail</t>
   </si>
   <si>
     <t xml:space="preserve">Reorder linked list</t>
@@ -949,32 +961,32 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1100,8 +1112,8 @@
   </sheetPr>
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K47" activeCellId="0" sqref="K47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J46" activeCellId="0" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2244,100 +2256,112 @@
       <c r="Q43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="77" t="n">
+      <c r="A44" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="B44" s="77" t="s">
+      <c r="B44" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C44" s="77"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="7"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="17"/>
+      <c r="H44" s="77" t="s">
+        <v>95</v>
+      </c>
+      <c r="I44" s="77"/>
+      <c r="J44" s="77"/>
+      <c r="K44" s="77"/>
+      <c r="L44" s="77"/>
+      <c r="M44" s="77"/>
+      <c r="N44" s="77"/>
+      <c r="O44" s="77"/>
+      <c r="P44" s="77"/>
       <c r="Q44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="79" t="n">
+      <c r="A45" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="B45" s="79" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="79"/>
-      <c r="D45" s="17"/>
+      <c r="B45" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="27"/>
+      <c r="D45" s="17" t="s">
+        <v>97</v>
+      </c>
       <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
+      <c r="F45" s="17" t="s">
+        <v>98</v>
+      </c>
       <c r="G45" s="17"/>
-      <c r="H45" s="80"/>
-      <c r="I45" s="80"/>
-      <c r="J45" s="80"/>
-      <c r="K45" s="80"/>
-      <c r="L45" s="80"/>
-      <c r="M45" s="80"/>
-      <c r="N45" s="80"/>
-      <c r="O45" s="80"/>
-      <c r="P45" s="80"/>
+      <c r="H45" s="77" t="s">
+        <v>99</v>
+      </c>
+      <c r="I45" s="77"/>
+      <c r="J45" s="77"/>
+      <c r="K45" s="77"/>
+      <c r="L45" s="77"/>
+      <c r="M45" s="77"/>
+      <c r="N45" s="77"/>
+      <c r="O45" s="77"/>
+      <c r="P45" s="77"/>
       <c r="Q45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="79" t="n">
+      <c r="A46" s="78" t="n">
         <v>3</v>
       </c>
-      <c r="B46" s="79" t="s">
-        <v>96</v>
-      </c>
-      <c r="C46" s="79"/>
+      <c r="B46" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="78"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
-      <c r="H46" s="81"/>
-      <c r="I46" s="82"/>
-      <c r="J46" s="82"/>
-      <c r="K46" s="82"/>
-      <c r="L46" s="82"/>
-      <c r="M46" s="82"/>
-      <c r="N46" s="82"/>
-      <c r="O46" s="82"/>
-      <c r="P46" s="82"/>
+      <c r="H46" s="79"/>
+      <c r="I46" s="80"/>
+      <c r="J46" s="80"/>
+      <c r="K46" s="80"/>
+      <c r="L46" s="80"/>
+      <c r="M46" s="80"/>
+      <c r="N46" s="80"/>
+      <c r="O46" s="80"/>
+      <c r="P46" s="80"/>
       <c r="Q46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="77" t="n">
+      <c r="A47" s="81" t="n">
         <v>4</v>
       </c>
-      <c r="B47" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="77"/>
+      <c r="B47" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="81"/>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
-      <c r="H47" s="81"/>
-      <c r="I47" s="81"/>
-      <c r="J47" s="81"/>
-      <c r="K47" s="81"/>
-      <c r="L47" s="81"/>
-      <c r="M47" s="81"/>
-      <c r="N47" s="81"/>
-      <c r="O47" s="81"/>
-      <c r="P47" s="81"/>
+      <c r="H47" s="79"/>
+      <c r="I47" s="79"/>
+      <c r="J47" s="79"/>
+      <c r="K47" s="79"/>
+      <c r="L47" s="79"/>
+      <c r="M47" s="79"/>
+      <c r="N47" s="79"/>
+      <c r="O47" s="79"/>
+      <c r="P47" s="79"/>
       <c r="Q47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -2345,28 +2369,28 @@
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
-      <c r="H48" s="83"/>
-      <c r="I48" s="83"/>
-      <c r="J48" s="83"/>
-      <c r="K48" s="83"/>
-      <c r="L48" s="83"/>
-      <c r="M48" s="83"/>
-      <c r="N48" s="83"/>
-      <c r="O48" s="83"/>
-      <c r="P48" s="83"/>
+      <c r="H48" s="82"/>
+      <c r="I48" s="82"/>
+      <c r="J48" s="82"/>
+      <c r="K48" s="82"/>
+      <c r="L48" s="82"/>
+      <c r="M48" s="82"/>
+      <c r="N48" s="82"/>
+      <c r="O48" s="82"/>
+      <c r="P48" s="82"/>
       <c r="Q48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="77" t="n">
+      <c r="A49" s="81" t="n">
         <v>1</v>
       </c>
-      <c r="B49" s="77" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="77"/>
-      <c r="D49" s="78"/>
-      <c r="E49" s="78"/>
-      <c r="F49" s="78"/>
+      <c r="B49" s="81" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="81"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="83"/>
+      <c r="F49" s="83"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
@@ -2380,16 +2404,16 @@
       <c r="Q49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="79" t="n">
+      <c r="A50" s="78" t="n">
         <v>2</v>
       </c>
-      <c r="B50" s="77" t="s">
-        <v>100</v>
-      </c>
-      <c r="C50" s="77"/>
-      <c r="D50" s="78"/>
-      <c r="E50" s="78"/>
-      <c r="F50" s="78"/>
+      <c r="B50" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" s="81"/>
+      <c r="D50" s="83"/>
+      <c r="E50" s="83"/>
+      <c r="F50" s="83"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
@@ -2407,7 +2431,7 @@
         <v>3</v>
       </c>
       <c r="B51" s="85" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C51" s="85"/>
       <c r="D51" s="34"/>
@@ -2423,12 +2447,12 @@
         <v>4</v>
       </c>
       <c r="B52" s="59" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C52" s="59"/>
-      <c r="D52" s="78"/>
-      <c r="E52" s="78"/>
-      <c r="F52" s="78"/>
+      <c r="D52" s="83"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="83"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
@@ -2436,13 +2460,13 @@
     </row>
     <row r="53" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="42" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B53" s="42"/>
       <c r="C53" s="42"/>
-      <c r="D53" s="78"/>
-      <c r="E53" s="78"/>
-      <c r="F53" s="78"/>
+      <c r="D53" s="83"/>
+      <c r="E53" s="83"/>
+      <c r="F53" s="83"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
@@ -2464,9 +2488,9 @@
       <c r="A55" s="87"/>
       <c r="B55" s="87"/>
       <c r="C55" s="87"/>
-      <c r="D55" s="78"/>
-      <c r="E55" s="78"/>
-      <c r="F55" s="78"/>
+      <c r="D55" s="83"/>
+      <c r="E55" s="83"/>
+      <c r="F55" s="83"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
@@ -2474,13 +2498,13 @@
     </row>
     <row r="56" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="12" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
-      <c r="D56" s="78"/>
-      <c r="E56" s="78"/>
-      <c r="F56" s="78"/>
+      <c r="D56" s="83"/>
+      <c r="E56" s="83"/>
+      <c r="F56" s="83"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
@@ -2502,9 +2526,9 @@
       <c r="A58" s="87"/>
       <c r="B58" s="87"/>
       <c r="C58" s="87"/>
-      <c r="D58" s="78"/>
-      <c r="E58" s="78"/>
-      <c r="F58" s="78"/>
+      <c r="D58" s="83"/>
+      <c r="E58" s="83"/>
+      <c r="F58" s="83"/>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
@@ -2512,13 +2536,13 @@
     </row>
     <row r="59" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="12" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
-      <c r="D59" s="78"/>
-      <c r="E59" s="78"/>
-      <c r="F59" s="78"/>
+      <c r="D59" s="83"/>
+      <c r="E59" s="83"/>
+      <c r="F59" s="83"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
@@ -2540,9 +2564,9 @@
       <c r="A61" s="87"/>
       <c r="B61" s="87"/>
       <c r="C61" s="87"/>
-      <c r="D61" s="78"/>
-      <c r="E61" s="78"/>
-      <c r="F61" s="78"/>
+      <c r="D61" s="83"/>
+      <c r="E61" s="83"/>
+      <c r="F61" s="83"/>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
@@ -2550,13 +2574,13 @@
     </row>
     <row r="62" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="12" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
-      <c r="D62" s="78"/>
-      <c r="E62" s="78"/>
-      <c r="F62" s="78"/>
+      <c r="D62" s="83"/>
+      <c r="E62" s="83"/>
+      <c r="F62" s="83"/>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
@@ -2567,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="48" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C63" s="48"/>
       <c r="D63" s="35"/>
@@ -2591,7 +2615,7 @@
     </row>
     <row r="65" s="1" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="12" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
@@ -2631,13 +2655,13 @@
     </row>
     <row r="68" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="42" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B68" s="42"/>
       <c r="C68" s="42"/>
-      <c r="D68" s="78"/>
-      <c r="E68" s="78"/>
-      <c r="F68" s="78"/>
+      <c r="D68" s="83"/>
+      <c r="E68" s="83"/>
+      <c r="F68" s="83"/>
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
@@ -2649,12 +2673,12 @@
         <v>1</v>
       </c>
       <c r="B69" s="91" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C69" s="91"/>
-      <c r="D69" s="78"/>
-      <c r="E69" s="78"/>
-      <c r="F69" s="78"/>
+      <c r="D69" s="83"/>
+      <c r="E69" s="83"/>
+      <c r="F69" s="83"/>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
@@ -2666,7 +2690,7 @@
         <v>2</v>
       </c>
       <c r="B70" s="93" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C70" s="93"/>
       <c r="D70" s="35"/>
@@ -2683,7 +2707,7 @@
         <v>3</v>
       </c>
       <c r="B71" s="93" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C71" s="93"/>
       <c r="D71" s="7"/>
@@ -2697,7 +2721,7 @@
     </row>
     <row r="72" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="12" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
@@ -2738,7 +2762,7 @@
     </row>
     <row r="75" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="12" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
@@ -2756,7 +2780,7 @@
         <v>1</v>
       </c>
       <c r="B76" s="94" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C76" s="94"/>
       <c r="D76" s="35"/>
@@ -2783,7 +2807,7 @@
     </row>
     <row r="78" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="12" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
@@ -2815,14 +2839,14 @@
     </row>
     <row r="81" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="12" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
     </row>
     <row r="84" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="42" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B84" s="42"/>
       <c r="C84" s="42"/>
@@ -2838,7 +2862,7 @@
       <c r="C86" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="166">
+  <mergeCells count="170">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
@@ -2975,9 +2999,13 @@
     <mergeCell ref="H42:P42"/>
     <mergeCell ref="A43:C43"/>
     <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:P44"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:P45"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="F46:G46"/>

</xml_diff>